<commit_message>
Added recording of registry studies and HTA
</commit_message>
<xml_diff>
--- a/data/seminars.xlsx
+++ b/data/seminars.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1209" uniqueCount="1032">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1210" uniqueCount="1033">
   <si>
     <t>Anja Schiel</t>
   </si>
@@ -3115,6 +3115,9 @@
   </si>
   <si>
     <t>6_DiBidino.pdf</t>
+  </si>
+  <si>
+    <t>https://streamingmedia.roche.com/media/t/1_yynoypov</t>
   </si>
 </sst>
 </file>
@@ -3575,9 +3578,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K995"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J1" sqref="J1"/>
+      <selection pane="bottomLeft" activeCell="C2" activeCellId="1" sqref="C2 C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3636,7 +3639,9 @@
       <c r="B2" s="3" t="s">
         <v>1004</v>
       </c>
-      <c r="C2" s="4"/>
+      <c r="C2" s="4" t="s">
+        <v>1032</v>
+      </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
       <c r="F2" s="1">
@@ -3703,7 +3708,7 @@
         <v>1027</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="28" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" ht="42" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
         <v>1003</v>
       </c>

</xml_diff>

<commit_message>
Upload slides and add time stamps to link to recording for joint BES/BBS seminar Real-World Data Quality – Assessing data quality and demonstrating fitness-for-purpose
</commit_message>
<xml_diff>
--- a/data/seminars.xlsx
+++ b/data/seminars.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1350" uniqueCount="1129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1355" uniqueCount="1134">
   <si>
     <t>Anja Schiel</t>
   </si>
@@ -3360,52 +3360,67 @@
     <t>https://streamingmedia.roche.com/media/t/1_xg0j74n0</t>
   </si>
   <si>
-    <t>Massoud Toussi</t>
-  </si>
-  <si>
     <t>IQVIA</t>
   </si>
   <si>
     <t>What is data quality, and how data types differ in terms of data quality</t>
   </si>
   <si>
-    <t>Nicole Mahoney</t>
-  </si>
-  <si>
     <t>RWD for regulatory decisions</t>
   </si>
   <si>
-    <t>Clair Blacketer</t>
-  </si>
-  <si>
     <t>EHDEN: Data Quality Dashboard</t>
   </si>
   <si>
-    <t>Daniel Morales</t>
-  </si>
-  <si>
     <t>EU Data quality framework</t>
   </si>
   <si>
-    <t>Dalia Dawoud</t>
-  </si>
-  <si>
     <t>COPD case study - The Use of the OMOP Common Data Model in Health Technology Assessment</t>
   </si>
   <si>
-    <t>Spencer James</t>
-  </si>
-  <si>
     <t>Roche/Genentech</t>
   </si>
   <si>
     <t>Data quality in Flatiron</t>
   </si>
   <si>
-    <t>Gracy Crane</t>
-  </si>
-  <si>
     <t>Transcelerate - How to bridge from framework to fitness for purpose demonstration?</t>
+  </si>
+  <si>
+    <t>Massoud Toussi (starts at 5:38)</t>
+  </si>
+  <si>
+    <t>Nicole Mahoney (25:35)</t>
+  </si>
+  <si>
+    <t>Clair Blacketer (39:48)</t>
+  </si>
+  <si>
+    <t>Daniel Morales (59:40)</t>
+  </si>
+  <si>
+    <t>Dalia Dawoud (1:18:43)</t>
+  </si>
+  <si>
+    <t>Spencer James (1:41:34)</t>
+  </si>
+  <si>
+    <t>Gracy Crane (NB this talk in the panel discussion section was not recorded, but the slides are attached)</t>
+  </si>
+  <si>
+    <t>1_Toussi.pdf</t>
+  </si>
+  <si>
+    <t>2_Mahoney.pdf</t>
+  </si>
+  <si>
+    <t>3_Blacketer.pdf</t>
+  </si>
+  <si>
+    <t>5_Dawoud.pdf</t>
+  </si>
+  <si>
+    <t>7_Crane</t>
   </si>
 </sst>
 </file>
@@ -3876,9 +3891,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K1026"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I9" sqref="I9"/>
+      <selection pane="bottomLeft" activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3934,7 +3949,7 @@
     </row>
     <row r="2" spans="1:11" ht="28" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="str">
-        <f>"15.03.2023"</f>
+        <f t="shared" ref="A2:A8" si="0">"15.03.2023"</f>
         <v>15.03.2023</v>
       </c>
       <c r="B2" s="3" t="s">
@@ -3949,19 +3964,21 @@
         <v>1</v>
       </c>
       <c r="G2" s="21" t="s">
+        <v>1122</v>
+      </c>
+      <c r="H2" s="21" t="s">
         <v>1113</v>
       </c>
-      <c r="H2" s="21" t="s">
+      <c r="I2" s="21" t="s">
         <v>1114</v>
       </c>
-      <c r="I2" s="21" t="s">
-        <v>1115</v>
-      </c>
-      <c r="J2" s="2"/>
+      <c r="J2" s="2" t="s">
+        <v>1129</v>
+      </c>
     </row>
     <row r="3" spans="1:11" ht="28" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="str">
-        <f>"15.03.2023"</f>
+        <f t="shared" si="0"/>
         <v>15.03.2023</v>
       </c>
       <c r="B3" s="3" t="s">
@@ -3974,19 +3991,21 @@
         <v>2</v>
       </c>
       <c r="G3" s="21" t="s">
-        <v>1116</v>
+        <v>1123</v>
       </c>
       <c r="H3" s="21" t="s">
         <v>897</v>
       </c>
       <c r="I3" s="21" t="s">
-        <v>1117</v>
-      </c>
-      <c r="J3" s="2"/>
+        <v>1115</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>1130</v>
+      </c>
     </row>
     <row r="4" spans="1:11" ht="28" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="str">
-        <f>"15.03.2023"</f>
+        <f t="shared" si="0"/>
         <v>15.03.2023</v>
       </c>
       <c r="B4" s="3" t="s">
@@ -3999,19 +4018,21 @@
         <v>3</v>
       </c>
       <c r="G4" s="21" t="s">
-        <v>1118</v>
+        <v>1124</v>
       </c>
       <c r="H4" s="21" t="s">
         <v>17</v>
       </c>
       <c r="I4" s="21" t="s">
-        <v>1119</v>
-      </c>
-      <c r="J4" s="2"/>
+        <v>1116</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>1131</v>
+      </c>
     </row>
     <row r="5" spans="1:11" ht="28" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="str">
-        <f>"15.03.2023"</f>
+        <f t="shared" si="0"/>
         <v>15.03.2023</v>
       </c>
       <c r="B5" s="3" t="s">
@@ -4024,19 +4045,19 @@
         <v>4</v>
       </c>
       <c r="G5" s="21" t="s">
-        <v>1120</v>
+        <v>1125</v>
       </c>
       <c r="H5" s="4" t="s">
         <v>261</v>
       </c>
       <c r="I5" s="21" t="s">
-        <v>1121</v>
+        <v>1117</v>
       </c>
       <c r="J5" s="2"/>
     </row>
     <row r="6" spans="1:11" ht="28" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="str">
-        <f>"15.03.2023"</f>
+        <f t="shared" si="0"/>
         <v>15.03.2023</v>
       </c>
       <c r="B6" s="3" t="s">
@@ -4049,19 +4070,21 @@
         <v>5</v>
       </c>
       <c r="G6" s="21" t="s">
-        <v>1122</v>
+        <v>1126</v>
       </c>
       <c r="H6" s="21" t="s">
         <v>956</v>
       </c>
       <c r="I6" s="21" t="s">
-        <v>1123</v>
-      </c>
-      <c r="J6" s="2"/>
+        <v>1118</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>1132</v>
+      </c>
     </row>
     <row r="7" spans="1:11" ht="28" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="str">
-        <f>"15.03.2023"</f>
+        <f t="shared" si="0"/>
         <v>15.03.2023</v>
       </c>
       <c r="B7" s="3" t="s">
@@ -4074,19 +4097,19 @@
         <v>6</v>
       </c>
       <c r="G7" s="21" t="s">
-        <v>1124</v>
+        <v>1127</v>
       </c>
       <c r="H7" s="21" t="s">
-        <v>1125</v>
+        <v>1119</v>
       </c>
       <c r="I7" s="21" t="s">
-        <v>1126</v>
+        <v>1120</v>
       </c>
       <c r="J7" s="2"/>
     </row>
     <row r="8" spans="1:11" ht="28" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="str">
-        <f>"15.03.2023"</f>
+        <f t="shared" si="0"/>
         <v>15.03.2023</v>
       </c>
       <c r="B8" s="3" t="s">
@@ -4099,15 +4122,17 @@
         <v>7</v>
       </c>
       <c r="G8" s="21" t="s">
-        <v>1127</v>
+        <v>1128</v>
       </c>
       <c r="H8" s="4" t="s">
         <v>1032</v>
       </c>
       <c r="I8" s="21" t="s">
-        <v>1128</v>
-      </c>
-      <c r="J8" s="2"/>
+        <v>1121</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>1133</v>
+      </c>
     </row>
     <row r="9" spans="1:11" ht="56" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="str">
@@ -4142,7 +4167,7 @@
     </row>
     <row r="10" spans="1:11" ht="56" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="str">
-        <f t="shared" ref="A10:A15" si="0">"15.12.2022"</f>
+        <f t="shared" ref="A10:A15" si="1">"15.12.2022"</f>
         <v>15.12.2022</v>
       </c>
       <c r="B10" s="3" t="s">
@@ -4169,7 +4194,7 @@
     </row>
     <row r="11" spans="1:11" ht="56" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>15.12.2022</v>
       </c>
       <c r="B11" s="3" t="s">
@@ -4196,7 +4221,7 @@
     </row>
     <row r="12" spans="1:11" ht="56" x14ac:dyDescent="0.35">
       <c r="A12" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>15.12.2022</v>
       </c>
       <c r="B12" s="3" t="s">
@@ -4223,7 +4248,7 @@
     </row>
     <row r="13" spans="1:11" ht="56" x14ac:dyDescent="0.35">
       <c r="A13" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>15.12.2022</v>
       </c>
       <c r="B13" s="3" t="s">
@@ -4250,7 +4275,7 @@
     </row>
     <row r="14" spans="1:11" ht="56" x14ac:dyDescent="0.35">
       <c r="A14" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>15.12.2022</v>
       </c>
       <c r="B14" s="3" t="s">
@@ -4277,7 +4302,7 @@
     </row>
     <row r="15" spans="1:11" ht="56" x14ac:dyDescent="0.35">
       <c r="A15" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>15.12.2022</v>
       </c>
       <c r="B15" s="3" t="s">
@@ -4302,7 +4327,7 @@
     </row>
     <row r="16" spans="1:11" ht="56" x14ac:dyDescent="0.35">
       <c r="A16" s="5" t="str">
-        <f t="shared" ref="A16:A21" si="1">"08.12.2022"</f>
+        <f t="shared" ref="A16:A21" si="2">"08.12.2022"</f>
         <v>08.12.2022</v>
       </c>
       <c r="B16" s="3" t="s">
@@ -4333,7 +4358,7 @@
     </row>
     <row r="17" spans="1:11" ht="56" x14ac:dyDescent="0.35">
       <c r="A17" s="5" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>08.12.2022</v>
       </c>
       <c r="B17" s="3" t="s">
@@ -4360,7 +4385,7 @@
     </row>
     <row r="18" spans="1:11" ht="56" x14ac:dyDescent="0.35">
       <c r="A18" s="5" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>08.12.2022</v>
       </c>
       <c r="B18" s="3" t="s">
@@ -4387,7 +4412,7 @@
     </row>
     <row r="19" spans="1:11" ht="56" x14ac:dyDescent="0.35">
       <c r="A19" s="5" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>08.12.2022</v>
       </c>
       <c r="B19" s="3" t="s">
@@ -4415,7 +4440,7 @@
     </row>
     <row r="20" spans="1:11" ht="56" x14ac:dyDescent="0.35">
       <c r="A20" s="5" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>08.12.2022</v>
       </c>
       <c r="B20" s="3" t="s">
@@ -4442,7 +4467,7 @@
     </row>
     <row r="21" spans="1:11" ht="56" x14ac:dyDescent="0.35">
       <c r="A21" s="5" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>08.12.2022</v>
       </c>
       <c r="B21" s="3" t="s">
@@ -4521,7 +4546,7 @@
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A24" s="5" t="str">
-        <f t="shared" ref="A24:A26" si="2">"30.11.2022"</f>
+        <f t="shared" ref="A24:A26" si="3">"30.11.2022"</f>
         <v>30.11.2022</v>
       </c>
       <c r="B24" s="3" t="s">
@@ -4546,7 +4571,7 @@
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A25" s="5" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>30.11.2022</v>
       </c>
       <c r="B25" s="3" t="s">
@@ -4571,7 +4596,7 @@
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A26" s="5" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>30.11.2022</v>
       </c>
       <c r="B26" s="3" t="s">
@@ -4596,7 +4621,7 @@
     </row>
     <row r="27" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A27" s="18" t="str">
-        <f t="shared" ref="A27:A32" si="3">"15.07.2022"</f>
+        <f t="shared" ref="A27:A32" si="4">"15.07.2022"</f>
         <v>15.07.2022</v>
       </c>
       <c r="B27" s="15" t="s">
@@ -4625,7 +4650,7 @@
     </row>
     <row r="28" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A28" s="18" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>15.07.2022</v>
       </c>
       <c r="B28" s="15" t="s">
@@ -4652,7 +4677,7 @@
     </row>
     <row r="29" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A29" s="18" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>15.07.2022</v>
       </c>
       <c r="B29" s="15" t="s">
@@ -4679,7 +4704,7 @@
     </row>
     <row r="30" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A30" s="18" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>15.07.2022</v>
       </c>
       <c r="B30" s="15" t="s">
@@ -4706,7 +4731,7 @@
     </row>
     <row r="31" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A31" s="18" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>15.07.2022</v>
       </c>
       <c r="B31" s="15" t="s">
@@ -4733,7 +4758,7 @@
     </row>
     <row r="32" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A32" s="18" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>15.07.2022</v>
       </c>
       <c r="B32" s="15" t="s">
@@ -4783,7 +4808,7 @@
     </row>
     <row r="34" spans="1:10" ht="56" x14ac:dyDescent="0.35">
       <c r="A34" s="18" t="str">
-        <f t="shared" ref="A34:A40" si="4">"23.06.2022"</f>
+        <f t="shared" ref="A34:A40" si="5">"23.06.2022"</f>
         <v>23.06.2022</v>
       </c>
       <c r="B34" s="3" t="s">
@@ -4808,7 +4833,7 @@
     </row>
     <row r="35" spans="1:10" ht="28" x14ac:dyDescent="0.35">
       <c r="A35" s="18" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>23.06.2022</v>
       </c>
       <c r="B35" s="3" t="s">
@@ -4835,7 +4860,7 @@
     </row>
     <row r="36" spans="1:10" ht="42" x14ac:dyDescent="0.35">
       <c r="A36" s="18" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>23.06.2022</v>
       </c>
       <c r="B36" s="3" t="s">
@@ -4862,7 +4887,7 @@
     </row>
     <row r="37" spans="1:10" ht="28" x14ac:dyDescent="0.35">
       <c r="A37" s="18" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>23.06.2022</v>
       </c>
       <c r="B37" s="3" t="s">
@@ -4889,7 +4914,7 @@
     </row>
     <row r="38" spans="1:10" ht="28" x14ac:dyDescent="0.35">
       <c r="A38" s="18" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>23.06.2022</v>
       </c>
       <c r="B38" s="3" t="s">
@@ -4916,7 +4941,7 @@
     </row>
     <row r="39" spans="1:10" ht="28" x14ac:dyDescent="0.35">
       <c r="A39" s="18" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>23.06.2022</v>
       </c>
       <c r="B39" s="3" t="s">
@@ -4943,7 +4968,7 @@
     </row>
     <row r="40" spans="1:10" ht="56" x14ac:dyDescent="0.35">
       <c r="A40" s="18" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>23.06.2022</v>
       </c>
       <c r="B40" s="3" t="s">
@@ -5103,7 +5128,7 @@
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A46" s="5" t="str">
-        <f t="shared" ref="A46:A48" si="5">"21.02.2022"</f>
+        <f t="shared" ref="A46:A48" si="6">"21.02.2022"</f>
         <v>21.02.2022</v>
       </c>
       <c r="B46" s="3"/>
@@ -5128,7 +5153,7 @@
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A47" s="5" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>21.02.2022</v>
       </c>
       <c r="B47" s="3"/>
@@ -5153,7 +5178,7 @@
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A48" s="5" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>21.02.2022</v>
       </c>
       <c r="B48" s="3"/>
@@ -5205,7 +5230,7 @@
     </row>
     <row r="50" spans="1:10" ht="42" x14ac:dyDescent="0.35">
       <c r="A50" s="9" t="str">
-        <f t="shared" ref="A50:A53" si="6">"27.07.2021"</f>
+        <f t="shared" ref="A50:A53" si="7">"27.07.2021"</f>
         <v>27.07.2021</v>
       </c>
       <c r="B50" s="13"/>
@@ -5230,7 +5255,7 @@
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A51" s="9" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>27.07.2021</v>
       </c>
       <c r="B51" s="13"/>
@@ -5255,7 +5280,7 @@
     </row>
     <row r="52" spans="1:10" ht="42" x14ac:dyDescent="0.35">
       <c r="A52" s="9" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>27.07.2021</v>
       </c>
       <c r="B52" s="13"/>
@@ -5280,7 +5305,7 @@
     </row>
     <row r="53" spans="1:10" ht="28" x14ac:dyDescent="0.35">
       <c r="A53" s="9" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>27.07.2021</v>
       </c>
       <c r="B53" s="13"/>
@@ -5334,7 +5359,7 @@
     </row>
     <row r="55" spans="1:10" ht="42" x14ac:dyDescent="0.35">
       <c r="A55" s="9" t="str">
-        <f t="shared" ref="A55:A61" si="7">"28.06.2021"</f>
+        <f t="shared" ref="A55:A61" si="8">"28.06.2021"</f>
         <v>28.06.2021</v>
       </c>
       <c r="B55" s="13"/>
@@ -5359,7 +5384,7 @@
     </row>
     <row r="56" spans="1:10" ht="28" x14ac:dyDescent="0.35">
       <c r="A56" s="9" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>28.06.2021</v>
       </c>
       <c r="B56" s="13"/>
@@ -5384,7 +5409,7 @@
     </row>
     <row r="57" spans="1:10" ht="42" x14ac:dyDescent="0.35">
       <c r="A57" s="9" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>28.06.2021</v>
       </c>
       <c r="B57" s="13"/>
@@ -5409,7 +5434,7 @@
     </row>
     <row r="58" spans="1:10" ht="28" x14ac:dyDescent="0.35">
       <c r="A58" s="9" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>28.06.2021</v>
       </c>
       <c r="B58" s="13"/>
@@ -5434,7 +5459,7 @@
     </row>
     <row r="59" spans="1:10" ht="42" x14ac:dyDescent="0.35">
       <c r="A59" s="9" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>28.06.2021</v>
       </c>
       <c r="B59" s="13"/>
@@ -5459,7 +5484,7 @@
     </row>
     <row r="60" spans="1:10" ht="42" x14ac:dyDescent="0.35">
       <c r="A60" s="9" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>28.06.2021</v>
       </c>
       <c r="B60" s="13"/>
@@ -5484,7 +5509,7 @@
     </row>
     <row r="61" spans="1:10" ht="56" x14ac:dyDescent="0.35">
       <c r="A61" s="9" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>28.06.2021</v>
       </c>
       <c r="B61" s="13"/>
@@ -5538,7 +5563,7 @@
     </row>
     <row r="63" spans="1:10" ht="42" x14ac:dyDescent="0.35">
       <c r="A63" s="9" t="str">
-        <f t="shared" ref="A63:A65" si="8">"16.06.2021"</f>
+        <f t="shared" ref="A63:A65" si="9">"16.06.2021"</f>
         <v>16.06.2021</v>
       </c>
       <c r="B63" s="13"/>
@@ -5563,7 +5588,7 @@
     </row>
     <row r="64" spans="1:10" ht="28" x14ac:dyDescent="0.35">
       <c r="A64" s="9" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>16.06.2021</v>
       </c>
       <c r="B64" s="13"/>
@@ -5588,7 +5613,7 @@
     </row>
     <row r="65" spans="1:10" ht="42" x14ac:dyDescent="0.35">
       <c r="A65" s="9" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>16.06.2021</v>
       </c>
       <c r="B65" s="13"/>
@@ -5642,7 +5667,7 @@
     </row>
     <row r="67" spans="1:10" ht="28" x14ac:dyDescent="0.35">
       <c r="A67" s="9" t="str">
-        <f t="shared" ref="A67:A75" si="9">"22.03.2021"</f>
+        <f t="shared" ref="A67:A75" si="10">"22.03.2021"</f>
         <v>22.03.2021</v>
       </c>
       <c r="B67" s="13"/>
@@ -5667,7 +5692,7 @@
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A68" s="9" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>22.03.2021</v>
       </c>
       <c r="B68" s="13"/>
@@ -5692,7 +5717,7 @@
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A69" s="9" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>22.03.2021</v>
       </c>
       <c r="B69" s="13"/>
@@ -5717,7 +5742,7 @@
     </row>
     <row r="70" spans="1:10" ht="28" x14ac:dyDescent="0.35">
       <c r="A70" s="9" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>22.03.2021</v>
       </c>
       <c r="B70" s="13"/>
@@ -5742,7 +5767,7 @@
     </row>
     <row r="71" spans="1:10" ht="28" x14ac:dyDescent="0.35">
       <c r="A71" s="9" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>22.03.2021</v>
       </c>
       <c r="B71" s="13"/>
@@ -5767,7 +5792,7 @@
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A72" s="9" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>22.03.2021</v>
       </c>
       <c r="B72" s="13"/>
@@ -5792,7 +5817,7 @@
     </row>
     <row r="73" spans="1:10" ht="42" x14ac:dyDescent="0.35">
       <c r="A73" s="9" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>22.03.2021</v>
       </c>
       <c r="B73" s="13"/>
@@ -5817,7 +5842,7 @@
     </row>
     <row r="74" spans="1:10" ht="28" x14ac:dyDescent="0.35">
       <c r="A74" s="9" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>22.03.2021</v>
       </c>
       <c r="B74" s="13"/>
@@ -5842,7 +5867,7 @@
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A75" s="9" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>22.03.2021</v>
       </c>
       <c r="B75" s="13"/>
@@ -5894,7 +5919,7 @@
     </row>
     <row r="77" spans="1:10" ht="28" x14ac:dyDescent="0.35">
       <c r="A77" s="9" t="str">
-        <f t="shared" ref="A77:A82" si="10">"08.03.2021"</f>
+        <f t="shared" ref="A77:A82" si="11">"08.03.2021"</f>
         <v>08.03.2021</v>
       </c>
       <c r="B77" s="13"/>
@@ -5919,7 +5944,7 @@
     </row>
     <row r="78" spans="1:10" ht="56" x14ac:dyDescent="0.35">
       <c r="A78" s="9" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>08.03.2021</v>
       </c>
       <c r="B78" s="13"/>
@@ -5944,7 +5969,7 @@
     </row>
     <row r="79" spans="1:10" ht="28" x14ac:dyDescent="0.35">
       <c r="A79" s="9" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>08.03.2021</v>
       </c>
       <c r="B79" s="13"/>
@@ -5969,7 +5994,7 @@
     </row>
     <row r="80" spans="1:10" ht="42" x14ac:dyDescent="0.35">
       <c r="A80" s="9" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>08.03.2021</v>
       </c>
       <c r="B80" s="13"/>
@@ -5994,7 +6019,7 @@
     </row>
     <row r="81" spans="1:10" ht="42" x14ac:dyDescent="0.35">
       <c r="A81" s="9" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>08.03.2021</v>
       </c>
       <c r="B81" s="13"/>
@@ -6019,7 +6044,7 @@
     </row>
     <row r="82" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A82" s="9" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>08.03.2021</v>
       </c>
       <c r="B82" s="13"/>
@@ -6071,7 +6096,7 @@
     </row>
     <row r="84" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A84" s="9" t="str">
-        <f t="shared" ref="A84:A90" si="11">"03.11.2020"</f>
+        <f t="shared" ref="A84:A90" si="12">"03.11.2020"</f>
         <v>03.11.2020</v>
       </c>
       <c r="B84" s="13"/>
@@ -6096,7 +6121,7 @@
     </row>
     <row r="85" spans="1:10" ht="42" x14ac:dyDescent="0.35">
       <c r="A85" s="9" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>03.11.2020</v>
       </c>
       <c r="B85" s="13"/>
@@ -6121,7 +6146,7 @@
     </row>
     <row r="86" spans="1:10" ht="56" x14ac:dyDescent="0.35">
       <c r="A86" s="9" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>03.11.2020</v>
       </c>
       <c r="B86" s="13"/>
@@ -6146,7 +6171,7 @@
     </row>
     <row r="87" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A87" s="9" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>03.11.2020</v>
       </c>
       <c r="B87" s="13"/>
@@ -6171,7 +6196,7 @@
     </row>
     <row r="88" spans="1:10" ht="28" x14ac:dyDescent="0.35">
       <c r="A88" s="9" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>03.11.2020</v>
       </c>
       <c r="B88" s="13"/>
@@ -6196,7 +6221,7 @@
     </row>
     <row r="89" spans="1:10" ht="42" x14ac:dyDescent="0.35">
       <c r="A89" s="9" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>03.11.2020</v>
       </c>
       <c r="B89" s="13"/>
@@ -6221,7 +6246,7 @@
     </row>
     <row r="90" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A90" s="9" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>03.11.2020</v>
       </c>
       <c r="B90" s="13"/>
@@ -6275,7 +6300,7 @@
     </row>
     <row r="92" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A92" s="9" t="str">
-        <f t="shared" ref="A92:A100" si="12">"07.09.2020"</f>
+        <f t="shared" ref="A92:A100" si="13">"07.09.2020"</f>
         <v>07.09.2020</v>
       </c>
       <c r="B92" s="13"/>
@@ -6300,7 +6325,7 @@
     </row>
     <row r="93" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A93" s="9" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>07.09.2020</v>
       </c>
       <c r="B93" s="13"/>
@@ -6325,7 +6350,7 @@
     </row>
     <row r="94" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A94" s="9" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>07.09.2020</v>
       </c>
       <c r="B94" s="13"/>
@@ -6350,7 +6375,7 @@
     </row>
     <row r="95" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A95" s="9" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>07.09.2020</v>
       </c>
       <c r="B95" s="13"/>
@@ -6375,7 +6400,7 @@
     </row>
     <row r="96" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A96" s="9" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>07.09.2020</v>
       </c>
       <c r="B96" s="13"/>
@@ -6400,7 +6425,7 @@
     </row>
     <row r="97" spans="1:10" ht="58" x14ac:dyDescent="0.35">
       <c r="A97" s="9" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>07.09.2020</v>
       </c>
       <c r="B97" s="13"/>
@@ -6425,7 +6450,7 @@
     </row>
     <row r="98" spans="1:10" ht="42" x14ac:dyDescent="0.35">
       <c r="A98" s="9" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>07.09.2020</v>
       </c>
       <c r="B98" s="13"/>
@@ -6450,7 +6475,7 @@
     </row>
     <row r="99" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A99" s="9" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>07.09.2020</v>
       </c>
       <c r="B99" s="13"/>
@@ -6475,7 +6500,7 @@
     </row>
     <row r="100" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A100" s="9" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>07.09.2020</v>
       </c>
       <c r="B100" s="13"/>
@@ -6527,7 +6552,7 @@
     </row>
     <row r="102" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A102" s="9" t="str">
-        <f t="shared" ref="A102:A105" si="13">"30.06.2020"</f>
+        <f t="shared" ref="A102:A105" si="14">"30.06.2020"</f>
         <v>30.06.2020</v>
       </c>
       <c r="B102" s="13"/>
@@ -6552,7 +6577,7 @@
     </row>
     <row r="103" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A103" s="9" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>30.06.2020</v>
       </c>
       <c r="B103" s="13"/>
@@ -6577,7 +6602,7 @@
     </row>
     <row r="104" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A104" s="9" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>30.06.2020</v>
       </c>
       <c r="B104" s="13"/>
@@ -6602,7 +6627,7 @@
     </row>
     <row r="105" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A105" s="9" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>30.06.2020</v>
       </c>
       <c r="B105" s="13"/>
@@ -6656,7 +6681,7 @@
     </row>
     <row r="107" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A107" s="9" t="str">
-        <f t="shared" ref="A107:A112" si="14">"29.06.2020"</f>
+        <f t="shared" ref="A107:A112" si="15">"29.06.2020"</f>
         <v>29.06.2020</v>
       </c>
       <c r="B107" s="13"/>
@@ -6681,7 +6706,7 @@
     </row>
     <row r="108" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A108" s="9" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>29.06.2020</v>
       </c>
       <c r="B108" s="13"/>
@@ -6706,7 +6731,7 @@
     </row>
     <row r="109" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A109" s="9" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>29.06.2020</v>
       </c>
       <c r="B109" s="13"/>
@@ -6731,7 +6756,7 @@
     </row>
     <row r="110" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A110" s="9" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>29.06.2020</v>
       </c>
       <c r="B110" s="13"/>
@@ -6756,7 +6781,7 @@
     </row>
     <row r="111" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A111" s="9" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>29.06.2020</v>
       </c>
       <c r="B111" s="13"/>
@@ -6781,7 +6806,7 @@
     </row>
     <row r="112" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A112" s="9" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>29.06.2020</v>
       </c>
       <c r="B112" s="13"/>
@@ -6831,7 +6856,7 @@
     </row>
     <row r="114" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A114" s="9" t="str">
-        <f t="shared" ref="A114:A116" si="15">"03.06.2020"</f>
+        <f t="shared" ref="A114:A116" si="16">"03.06.2020"</f>
         <v>03.06.2020</v>
       </c>
       <c r="B114" s="13"/>
@@ -6856,7 +6881,7 @@
     </row>
     <row r="115" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A115" s="9" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>03.06.2020</v>
       </c>
       <c r="B115" s="13"/>
@@ -6881,7 +6906,7 @@
     </row>
     <row r="116" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A116" s="9" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>03.06.2020</v>
       </c>
       <c r="B116" s="13"/>
@@ -6933,7 +6958,7 @@
     </row>
     <row r="118" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A118" s="9" t="str">
-        <f t="shared" ref="A118:A122" si="16">"06.05.2020"</f>
+        <f t="shared" ref="A118:A122" si="17">"06.05.2020"</f>
         <v>06.05.2020</v>
       </c>
       <c r="B118" s="13"/>
@@ -6958,7 +6983,7 @@
     </row>
     <row r="119" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A119" s="9" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>06.05.2020</v>
       </c>
       <c r="B119" s="13"/>
@@ -6983,7 +7008,7 @@
     </row>
     <row r="120" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A120" s="9" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>06.05.2020</v>
       </c>
       <c r="B120" s="13"/>
@@ -7008,7 +7033,7 @@
     </row>
     <row r="121" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A121" s="9" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>06.05.2020</v>
       </c>
       <c r="B121" s="13"/>
@@ -7033,7 +7058,7 @@
     </row>
     <row r="122" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A122" s="9" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>06.05.2020</v>
       </c>
       <c r="B122" s="13"/>
@@ -7083,7 +7108,7 @@
     </row>
     <row r="124" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A124" s="9" t="str">
-        <f t="shared" ref="A124:A128" si="17">"04.02.2020"</f>
+        <f t="shared" ref="A124:A128" si="18">"04.02.2020"</f>
         <v>04.02.2020</v>
       </c>
       <c r="B124" s="13"/>
@@ -7106,7 +7131,7 @@
     </row>
     <row r="125" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A125" s="9" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>04.02.2020</v>
       </c>
       <c r="B125" s="13"/>
@@ -7129,7 +7154,7 @@
     </row>
     <row r="126" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A126" s="9" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>04.02.2020</v>
       </c>
       <c r="B126" s="13"/>
@@ -7152,7 +7177,7 @@
     </row>
     <row r="127" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A127" s="9" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>04.02.2020</v>
       </c>
       <c r="B127" s="13"/>
@@ -7173,7 +7198,7 @@
     </row>
     <row r="128" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A128" s="9" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>04.02.2020</v>
       </c>
       <c r="B128" s="13"/>
@@ -7221,7 +7246,7 @@
     </row>
     <row r="130" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A130" s="9" t="str">
-        <f t="shared" ref="A130:A137" si="18">"01.11.2019"</f>
+        <f t="shared" ref="A130:A137" si="19">"01.11.2019"</f>
         <v>01.11.2019</v>
       </c>
       <c r="B130" s="13"/>
@@ -7244,7 +7269,7 @@
     </row>
     <row r="131" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A131" s="9" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>01.11.2019</v>
       </c>
       <c r="B131" s="13"/>
@@ -7267,7 +7292,7 @@
     </row>
     <row r="132" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A132" s="9" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>01.11.2019</v>
       </c>
       <c r="B132" s="13"/>
@@ -7290,7 +7315,7 @@
     </row>
     <row r="133" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A133" s="9" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>01.11.2019</v>
       </c>
       <c r="B133" s="13"/>
@@ -7313,7 +7338,7 @@
     </row>
     <row r="134" spans="1:11" ht="58" x14ac:dyDescent="0.35">
       <c r="A134" s="9" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>01.11.2019</v>
       </c>
       <c r="B134" s="13"/>
@@ -7333,7 +7358,7 @@
     </row>
     <row r="135" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A135" s="9" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>01.11.2019</v>
       </c>
       <c r="B135" s="13"/>
@@ -7356,7 +7381,7 @@
     </row>
     <row r="136" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A136" s="9" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>01.11.2019</v>
       </c>
       <c r="B136" s="13"/>
@@ -7379,7 +7404,7 @@
     </row>
     <row r="137" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A137" s="9" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>01.11.2019</v>
       </c>
       <c r="B137" s="13"/>
@@ -7426,7 +7451,7 @@
     </row>
     <row r="139" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A139" s="9" t="str">
-        <f t="shared" ref="A139:A144" si="19">"21.08.2019"</f>
+        <f t="shared" ref="A139:A144" si="20">"21.08.2019"</f>
         <v>21.08.2019</v>
       </c>
       <c r="B139" s="13"/>
@@ -7448,7 +7473,7 @@
     </row>
     <row r="140" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A140" s="9" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>21.08.2019</v>
       </c>
       <c r="B140" s="13"/>
@@ -7467,7 +7492,7 @@
     </row>
     <row r="141" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A141" s="9" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>21.08.2019</v>
       </c>
       <c r="B141" s="13"/>
@@ -7487,7 +7512,7 @@
     </row>
     <row r="142" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A142" s="9" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>21.08.2019</v>
       </c>
       <c r="B142" s="13"/>
@@ -7507,7 +7532,7 @@
     </row>
     <row r="143" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A143" s="9" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>21.08.2019</v>
       </c>
       <c r="B143" s="13"/>
@@ -7527,7 +7552,7 @@
     </row>
     <row r="144" spans="1:11" ht="58" x14ac:dyDescent="0.35">
       <c r="A144" s="9" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>21.08.2019</v>
       </c>
       <c r="B144" s="13"/>
@@ -7570,7 +7595,7 @@
     </row>
     <row r="146" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A146" s="9" t="str">
-        <f t="shared" ref="A146:A152" si="20">"04.06.2019"</f>
+        <f t="shared" ref="A146:A152" si="21">"04.06.2019"</f>
         <v>04.06.2019</v>
       </c>
       <c r="B146" s="13"/>
@@ -7592,7 +7617,7 @@
     </row>
     <row r="147" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A147" s="9" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>04.06.2019</v>
       </c>
       <c r="B147" s="13"/>
@@ -7614,7 +7639,7 @@
     </row>
     <row r="148" spans="1:10" ht="58" x14ac:dyDescent="0.35">
       <c r="A148" s="9" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>04.06.2019</v>
       </c>
       <c r="B148" s="13"/>
@@ -7636,7 +7661,7 @@
     </row>
     <row r="149" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A149" s="9" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>04.06.2019</v>
       </c>
       <c r="B149" s="13"/>
@@ -7658,7 +7683,7 @@
     </row>
     <row r="150" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A150" s="9" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>04.06.2019</v>
       </c>
       <c r="B150" s="13"/>
@@ -7680,7 +7705,7 @@
     </row>
     <row r="151" spans="1:10" ht="58" x14ac:dyDescent="0.35">
       <c r="A151" s="9" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>04.06.2019</v>
       </c>
       <c r="B151" s="13"/>
@@ -7702,7 +7727,7 @@
     </row>
     <row r="152" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A152" s="9" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>04.06.2019</v>
       </c>
       <c r="B152" s="13"/>
@@ -7748,7 +7773,7 @@
     </row>
     <row r="154" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A154" s="9" t="str">
-        <f t="shared" ref="A154:A164" si="21">"10.05.2019"</f>
+        <f t="shared" ref="A154:A164" si="22">"10.05.2019"</f>
         <v>10.05.2019</v>
       </c>
       <c r="B154" s="13"/>
@@ -7770,7 +7795,7 @@
     </row>
     <row r="155" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A155" s="9" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>10.05.2019</v>
       </c>
       <c r="B155" s="13"/>
@@ -7792,7 +7817,7 @@
     </row>
     <row r="156" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A156" s="9" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>10.05.2019</v>
       </c>
       <c r="B156" s="13"/>
@@ -7814,7 +7839,7 @@
     </row>
     <row r="157" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A157" s="9" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>10.05.2019</v>
       </c>
       <c r="B157" s="13"/>
@@ -7836,7 +7861,7 @@
     </row>
     <row r="158" spans="1:10" ht="58" x14ac:dyDescent="0.35">
       <c r="A158" s="9" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>10.05.2019</v>
       </c>
       <c r="B158" s="13"/>
@@ -7858,7 +7883,7 @@
     </row>
     <row r="159" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A159" s="9" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>10.05.2019</v>
       </c>
       <c r="B159" s="13"/>
@@ -7880,7 +7905,7 @@
     </row>
     <row r="160" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A160" s="9" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>10.05.2019</v>
       </c>
       <c r="B160" s="13"/>
@@ -7902,7 +7927,7 @@
     </row>
     <row r="161" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A161" s="9" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>10.05.2019</v>
       </c>
       <c r="B161" s="13"/>
@@ -7924,7 +7949,7 @@
     </row>
     <row r="162" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A162" s="9" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>10.05.2019</v>
       </c>
       <c r="B162" s="13"/>
@@ -7946,7 +7971,7 @@
     </row>
     <row r="163" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A163" s="9" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>10.05.2019</v>
       </c>
       <c r="B163" s="13"/>
@@ -7965,7 +7990,7 @@
     </row>
     <row r="164" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A164" s="9" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>10.05.2019</v>
       </c>
       <c r="B164" s="13"/>
@@ -8008,7 +8033,7 @@
     </row>
     <row r="166" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A166" s="9" t="str">
-        <f t="shared" ref="A166:A173" si="22">"27.06.2018"</f>
+        <f t="shared" ref="A166:A173" si="23">"27.06.2018"</f>
         <v>27.06.2018</v>
       </c>
       <c r="B166" s="13"/>
@@ -8030,7 +8055,7 @@
     </row>
     <row r="167" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A167" s="9" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>27.06.2018</v>
       </c>
       <c r="B167" s="13"/>
@@ -8052,7 +8077,7 @@
     </row>
     <row r="168" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A168" s="9" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>27.06.2018</v>
       </c>
       <c r="B168" s="13"/>
@@ -8074,7 +8099,7 @@
     </row>
     <row r="169" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A169" s="9" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>27.06.2018</v>
       </c>
       <c r="B169" s="13"/>
@@ -8096,7 +8121,7 @@
     </row>
     <row r="170" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A170" s="9" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>27.06.2018</v>
       </c>
       <c r="B170" s="13"/>
@@ -8118,7 +8143,7 @@
     </row>
     <row r="171" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A171" s="9" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>27.06.2018</v>
       </c>
       <c r="B171" s="13"/>
@@ -8140,7 +8165,7 @@
     </row>
     <row r="172" spans="1:10" ht="58" x14ac:dyDescent="0.35">
       <c r="A172" s="9" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>27.06.2018</v>
       </c>
       <c r="B172" s="13"/>
@@ -8162,7 +8187,7 @@
     </row>
     <row r="173" spans="1:10" ht="58" x14ac:dyDescent="0.35">
       <c r="A173" s="9" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>27.06.2018</v>
       </c>
       <c r="B173" s="13"/>
@@ -8208,7 +8233,7 @@
     </row>
     <row r="175" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A175" s="9" t="str">
-        <f t="shared" ref="A175:A176" si="23">"26.06.2018"</f>
+        <f t="shared" ref="A175:A176" si="24">"26.06.2018"</f>
         <v>26.06.2018</v>
       </c>
       <c r="B175" s="13"/>
@@ -8230,7 +8255,7 @@
     </row>
     <row r="176" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A176" s="9" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>26.06.2018</v>
       </c>
       <c r="B176" s="13"/>
@@ -8276,7 +8301,7 @@
     </row>
     <row r="178" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A178" s="9" t="str">
-        <f t="shared" ref="A178:A181" si="24">"17.04.2018"</f>
+        <f t="shared" ref="A178:A181" si="25">"17.04.2018"</f>
         <v>17.04.2018</v>
       </c>
       <c r="B178" s="13"/>
@@ -8298,7 +8323,7 @@
     </row>
     <row r="179" spans="1:10" ht="58" x14ac:dyDescent="0.35">
       <c r="A179" s="9" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>17.04.2018</v>
       </c>
       <c r="B179" s="13"/>
@@ -8320,7 +8345,7 @@
     </row>
     <row r="180" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A180" s="9" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>17.04.2018</v>
       </c>
       <c r="B180" s="13"/>
@@ -8342,7 +8367,7 @@
     </row>
     <row r="181" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A181" s="9" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>17.04.2018</v>
       </c>
       <c r="B181" s="13"/>
@@ -8388,7 +8413,7 @@
     </row>
     <row r="183" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A183" s="9" t="str">
-        <f t="shared" ref="A183:A184" si="25">"20.03.2018"</f>
+        <f t="shared" ref="A183:A184" si="26">"20.03.2018"</f>
         <v>20.03.2018</v>
       </c>
       <c r="B183" s="13"/>
@@ -8410,7 +8435,7 @@
     </row>
     <row r="184" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A184" s="9" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>20.03.2018</v>
       </c>
       <c r="B184" s="13"/>
@@ -8528,7 +8553,7 @@
     </row>
     <row r="189" spans="1:10" ht="28" x14ac:dyDescent="0.35">
       <c r="A189" s="9" t="str">
-        <f t="shared" ref="A189:A195" si="26">"11.09.2017"</f>
+        <f t="shared" ref="A189:A195" si="27">"11.09.2017"</f>
         <v>11.09.2017</v>
       </c>
       <c r="B189" s="13"/>
@@ -8551,7 +8576,7 @@
     </row>
     <row r="190" spans="1:10" ht="56" x14ac:dyDescent="0.35">
       <c r="A190" s="9" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>11.09.2017</v>
       </c>
       <c r="B190" s="13"/>
@@ -8574,7 +8599,7 @@
     </row>
     <row r="191" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A191" s="9" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>11.09.2017</v>
       </c>
       <c r="B191" s="13"/>
@@ -8597,7 +8622,7 @@
     </row>
     <row r="192" spans="1:10" ht="28" x14ac:dyDescent="0.35">
       <c r="A192" s="9" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>11.09.2017</v>
       </c>
       <c r="B192" s="13"/>
@@ -8620,7 +8645,7 @@
     </row>
     <row r="193" spans="1:10" ht="42" x14ac:dyDescent="0.35">
       <c r="A193" s="9" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>11.09.2017</v>
       </c>
       <c r="B193" s="13"/>
@@ -8643,7 +8668,7 @@
     </row>
     <row r="194" spans="1:10" ht="56" x14ac:dyDescent="0.35">
       <c r="A194" s="9" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>11.09.2017</v>
       </c>
       <c r="B194" s="13"/>
@@ -8666,7 +8691,7 @@
     </row>
     <row r="195" spans="1:10" ht="28" x14ac:dyDescent="0.35">
       <c r="A195" s="9" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>11.09.2017</v>
       </c>
       <c r="B195" s="13"/>
@@ -8714,7 +8739,7 @@
     </row>
     <row r="197" spans="1:10" ht="28" x14ac:dyDescent="0.35">
       <c r="A197" s="9" t="str">
-        <f t="shared" ref="A197:A198" si="27">"26.06.2017"</f>
+        <f t="shared" ref="A197:A198" si="28">"26.06.2017"</f>
         <v>26.06.2017</v>
       </c>
       <c r="B197" s="13"/>
@@ -8737,7 +8762,7 @@
     </row>
     <row r="198" spans="1:10" ht="28" x14ac:dyDescent="0.35">
       <c r="A198" s="9" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>26.06.2017</v>
       </c>
       <c r="B198" s="13"/>
@@ -8760,7 +8785,7 @@
     </row>
     <row r="199" spans="1:10" ht="42" x14ac:dyDescent="0.35">
       <c r="A199" s="9" t="str">
-        <f t="shared" ref="A199:A207" si="28">"15.06.2017"</f>
+        <f t="shared" ref="A199:A207" si="29">"15.06.2017"</f>
         <v>15.06.2017</v>
       </c>
       <c r="B199" s="13" t="s">
@@ -8784,7 +8809,7 @@
     </row>
     <row r="200" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A200" s="9" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>15.06.2017</v>
       </c>
       <c r="B200" s="13"/>
@@ -8806,7 +8831,7 @@
     </row>
     <row r="201" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A201" s="9" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>15.06.2017</v>
       </c>
       <c r="B201" s="13"/>
@@ -8828,7 +8853,7 @@
     </row>
     <row r="202" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A202" s="9" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>15.06.2017</v>
       </c>
       <c r="B202" s="13"/>
@@ -8850,7 +8875,7 @@
     </row>
     <row r="203" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A203" s="9" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>15.06.2017</v>
       </c>
       <c r="B203" s="13"/>
@@ -8872,7 +8897,7 @@
     </row>
     <row r="204" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A204" s="9" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>15.06.2017</v>
       </c>
       <c r="B204" s="13"/>
@@ -8894,7 +8919,7 @@
     </row>
     <row r="205" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A205" s="9" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>15.06.2017</v>
       </c>
       <c r="B205" s="13"/>
@@ -8916,7 +8941,7 @@
     </row>
     <row r="206" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A206" s="9" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>15.06.2017</v>
       </c>
       <c r="B206" s="13"/>
@@ -8938,7 +8963,7 @@
     </row>
     <row r="207" spans="1:10" ht="58" x14ac:dyDescent="0.35">
       <c r="A207" s="9" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>15.06.2017</v>
       </c>
       <c r="B207" s="13"/>
@@ -8984,7 +9009,7 @@
     </row>
     <row r="209" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A209" s="9" t="str">
-        <f t="shared" ref="A209:A213" si="29">"05.05.2017"</f>
+        <f t="shared" ref="A209:A213" si="30">"05.05.2017"</f>
         <v>05.05.2017</v>
       </c>
       <c r="B209" s="13"/>
@@ -9006,7 +9031,7 @@
     </row>
     <row r="210" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A210" s="9" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>05.05.2017</v>
       </c>
       <c r="B210" s="13"/>
@@ -9028,7 +9053,7 @@
     </row>
     <row r="211" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A211" s="9" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>05.05.2017</v>
       </c>
       <c r="B211" s="13"/>
@@ -9050,7 +9075,7 @@
     </row>
     <row r="212" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A212" s="9" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>05.05.2017</v>
       </c>
       <c r="B212" s="13"/>
@@ -9072,7 +9097,7 @@
     </row>
     <row r="213" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A213" s="9" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>05.05.2017</v>
       </c>
       <c r="B213" s="13"/>
@@ -9168,7 +9193,7 @@
     </row>
     <row r="217" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A217" s="9" t="str">
-        <f t="shared" ref="A217:A220" si="30">"29.11.2016"</f>
+        <f t="shared" ref="A217:A220" si="31">"29.11.2016"</f>
         <v>29.11.2016</v>
       </c>
       <c r="B217" s="13"/>
@@ -9190,7 +9215,7 @@
     </row>
     <row r="218" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A218" s="9" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>29.11.2016</v>
       </c>
       <c r="B218" s="13"/>
@@ -9212,7 +9237,7 @@
     </row>
     <row r="219" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A219" s="9" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>29.11.2016</v>
       </c>
       <c r="B219" s="13"/>
@@ -9234,7 +9259,7 @@
     </row>
     <row r="220" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A220" s="9" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>29.11.2016</v>
       </c>
       <c r="B220" s="13"/>
@@ -9281,7 +9306,7 @@
     </row>
     <row r="222" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A222" s="9" t="str">
-        <f t="shared" ref="A222:A224" si="31">"14.11.2016"</f>
+        <f t="shared" ref="A222:A224" si="32">"14.11.2016"</f>
         <v>14.11.2016</v>
       </c>
       <c r="B222" s="13"/>
@@ -9304,7 +9329,7 @@
     </row>
     <row r="223" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A223" s="9" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>14.11.2016</v>
       </c>
       <c r="B223" s="13"/>
@@ -9327,7 +9352,7 @@
     </row>
     <row r="224" spans="1:10" ht="58" x14ac:dyDescent="0.35">
       <c r="A224" s="9" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>14.11.2016</v>
       </c>
       <c r="B224" s="13"/>
@@ -9375,7 +9400,7 @@
     </row>
     <row r="226" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A226" s="9" t="str">
-        <f t="shared" ref="A226:A227" si="32">"17.10.2016"</f>
+        <f t="shared" ref="A226:A227" si="33">"17.10.2016"</f>
         <v>17.10.2016</v>
       </c>
       <c r="B226" s="13"/>
@@ -9398,7 +9423,7 @@
     </row>
     <row r="227" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A227" s="9" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>17.10.2016</v>
       </c>
       <c r="B227" s="13"/>
@@ -9446,7 +9471,7 @@
     </row>
     <row r="229" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A229" s="9" t="str">
-        <f t="shared" ref="A229:A233" si="33">"14.09.2016"</f>
+        <f t="shared" ref="A229:A233" si="34">"14.09.2016"</f>
         <v>14.09.2016</v>
       </c>
       <c r="B229" s="13"/>
@@ -9469,7 +9494,7 @@
     </row>
     <row r="230" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A230" s="9" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>14.09.2016</v>
       </c>
       <c r="B230" s="13"/>
@@ -9492,7 +9517,7 @@
     </row>
     <row r="231" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A231" s="9" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>14.09.2016</v>
       </c>
       <c r="B231" s="13"/>
@@ -9515,7 +9540,7 @@
     </row>
     <row r="232" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A232" s="9" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>14.09.2016</v>
       </c>
       <c r="B232" s="13"/>
@@ -9538,7 +9563,7 @@
     </row>
     <row r="233" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A233" s="9" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>14.09.2016</v>
       </c>
       <c r="B233" s="13"/>
@@ -9673,7 +9698,7 @@
     </row>
     <row r="239" spans="1:10" ht="28" x14ac:dyDescent="0.35">
       <c r="A239" s="9" t="str">
-        <f t="shared" ref="A239:A247" si="34">"28.04.2016"</f>
+        <f t="shared" ref="A239:A247" si="35">"28.04.2016"</f>
         <v>28.04.2016</v>
       </c>
       <c r="B239" s="13"/>
@@ -9696,7 +9721,7 @@
     </row>
     <row r="240" spans="1:10" ht="56" x14ac:dyDescent="0.35">
       <c r="A240" s="9" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>28.04.2016</v>
       </c>
       <c r="B240" s="13"/>
@@ -9716,7 +9741,7 @@
     </row>
     <row r="241" spans="1:10" ht="28" x14ac:dyDescent="0.35">
       <c r="A241" s="9" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>28.04.2016</v>
       </c>
       <c r="B241" s="13"/>
@@ -9739,7 +9764,7 @@
     </row>
     <row r="242" spans="1:10" ht="28" x14ac:dyDescent="0.35">
       <c r="A242" s="9" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>28.04.2016</v>
       </c>
       <c r="B242" s="13"/>
@@ -9762,7 +9787,7 @@
     </row>
     <row r="243" spans="1:10" ht="42" x14ac:dyDescent="0.35">
       <c r="A243" s="9" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>28.04.2016</v>
       </c>
       <c r="B243" s="13"/>
@@ -9785,7 +9810,7 @@
     </row>
     <row r="244" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A244" s="9" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>28.04.2016</v>
       </c>
       <c r="B244" s="13"/>
@@ -9808,7 +9833,7 @@
     </row>
     <row r="245" spans="1:10" ht="28" x14ac:dyDescent="0.35">
       <c r="A245" s="9" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>28.04.2016</v>
       </c>
       <c r="B245" s="13"/>
@@ -9829,7 +9854,7 @@
     </row>
     <row r="246" spans="1:10" ht="28" x14ac:dyDescent="0.35">
       <c r="A246" s="9" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>28.04.2016</v>
       </c>
       <c r="B246" s="13"/>
@@ -9852,7 +9877,7 @@
     </row>
     <row r="247" spans="1:10" ht="28" x14ac:dyDescent="0.35">
       <c r="A247" s="9" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>28.04.2016</v>
       </c>
       <c r="B247" s="13"/>
@@ -9898,7 +9923,7 @@
     </row>
     <row r="249" spans="1:10" ht="70" x14ac:dyDescent="0.35">
       <c r="A249" s="9" t="str">
-        <f t="shared" ref="A249:A253" si="35">"13.01.2016"</f>
+        <f t="shared" ref="A249:A253" si="36">"13.01.2016"</f>
         <v>13.01.2016</v>
       </c>
       <c r="B249" s="13"/>
@@ -9921,7 +9946,7 @@
     </row>
     <row r="250" spans="1:10" ht="28" x14ac:dyDescent="0.35">
       <c r="A250" s="9" t="str">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>13.01.2016</v>
       </c>
       <c r="B250" s="13"/>
@@ -9944,7 +9969,7 @@
     </row>
     <row r="251" spans="1:10" ht="28" x14ac:dyDescent="0.35">
       <c r="A251" s="9" t="str">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>13.01.2016</v>
       </c>
       <c r="B251" s="13"/>
@@ -9967,7 +9992,7 @@
     </row>
     <row r="252" spans="1:10" ht="28" x14ac:dyDescent="0.35">
       <c r="A252" s="9" t="str">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>13.01.2016</v>
       </c>
       <c r="B252" s="13"/>
@@ -9988,7 +10013,7 @@
     </row>
     <row r="253" spans="1:10" ht="56" x14ac:dyDescent="0.35">
       <c r="A253" s="9" t="str">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>13.01.2016</v>
       </c>
       <c r="B253" s="13"/>
@@ -10082,7 +10107,7 @@
     </row>
     <row r="257" spans="1:10" ht="56" x14ac:dyDescent="0.35">
       <c r="A257" s="9" t="str">
-        <f t="shared" ref="A257:A266" si="36">"23.06.2015"</f>
+        <f t="shared" ref="A257:A266" si="37">"23.06.2015"</f>
         <v>23.06.2015</v>
       </c>
       <c r="B257" s="13"/>
@@ -10103,7 +10128,7 @@
     </row>
     <row r="258" spans="1:10" ht="28" x14ac:dyDescent="0.35">
       <c r="A258" s="9" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>23.06.2015</v>
       </c>
       <c r="B258" s="13"/>
@@ -10126,7 +10151,7 @@
     </row>
     <row r="259" spans="1:10" ht="42" x14ac:dyDescent="0.35">
       <c r="A259" s="9" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>23.06.2015</v>
       </c>
       <c r="B259" s="13"/>
@@ -10149,7 +10174,7 @@
     </row>
     <row r="260" spans="1:10" ht="28" x14ac:dyDescent="0.35">
       <c r="A260" s="9" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>23.06.2015</v>
       </c>
       <c r="B260" s="13"/>
@@ -10172,7 +10197,7 @@
     </row>
     <row r="261" spans="1:10" ht="28" x14ac:dyDescent="0.35">
       <c r="A261" s="9" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>23.06.2015</v>
       </c>
       <c r="B261" s="13"/>
@@ -10195,7 +10220,7 @@
     </row>
     <row r="262" spans="1:10" ht="28" x14ac:dyDescent="0.35">
       <c r="A262" s="9" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>23.06.2015</v>
       </c>
       <c r="B262" s="13"/>
@@ -10218,7 +10243,7 @@
     </row>
     <row r="263" spans="1:10" ht="42" x14ac:dyDescent="0.35">
       <c r="A263" s="9" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>23.06.2015</v>
       </c>
       <c r="B263" s="13"/>
@@ -10241,7 +10266,7 @@
     </row>
     <row r="264" spans="1:10" ht="42" x14ac:dyDescent="0.35">
       <c r="A264" s="9" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>23.06.2015</v>
       </c>
       <c r="B264" s="13"/>
@@ -10264,7 +10289,7 @@
     </row>
     <row r="265" spans="1:10" ht="28" x14ac:dyDescent="0.35">
       <c r="A265" s="9" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>23.06.2015</v>
       </c>
       <c r="B265" s="13"/>
@@ -10287,7 +10312,7 @@
     </row>
     <row r="266" spans="1:10" ht="42" x14ac:dyDescent="0.35">
       <c r="A266" s="9" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>23.06.2015</v>
       </c>
       <c r="B266" s="13"/>
@@ -10406,7 +10431,7 @@
     </row>
     <row r="271" spans="1:10" ht="28" x14ac:dyDescent="0.35">
       <c r="A271" s="9" t="str">
-        <f t="shared" ref="A271:A277" si="37">"13.11.2014"</f>
+        <f t="shared" ref="A271:A277" si="38">"13.11.2014"</f>
         <v>13.11.2014</v>
       </c>
       <c r="B271" s="13"/>
@@ -10429,7 +10454,7 @@
     </row>
     <row r="272" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A272" s="9" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>13.11.2014</v>
       </c>
       <c r="B272" s="13"/>
@@ -10452,7 +10477,7 @@
     </row>
     <row r="273" spans="1:10" ht="28" x14ac:dyDescent="0.35">
       <c r="A273" s="9" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>13.11.2014</v>
       </c>
       <c r="B273" s="13"/>
@@ -10475,7 +10500,7 @@
     </row>
     <row r="274" spans="1:10" ht="28" x14ac:dyDescent="0.35">
       <c r="A274" s="9" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>13.11.2014</v>
       </c>
       <c r="B274" s="13"/>
@@ -10498,7 +10523,7 @@
     </row>
     <row r="275" spans="1:10" ht="28" x14ac:dyDescent="0.35">
       <c r="A275" s="9" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>13.11.2014</v>
       </c>
       <c r="B275" s="13"/>
@@ -10521,7 +10546,7 @@
     </row>
     <row r="276" spans="1:10" ht="28" x14ac:dyDescent="0.35">
       <c r="A276" s="9" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>13.11.2014</v>
       </c>
       <c r="B276" s="13"/>
@@ -10544,7 +10569,7 @@
     </row>
     <row r="277" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A277" s="9" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>13.11.2014</v>
       </c>
       <c r="B277" s="13"/>
@@ -10592,7 +10617,7 @@
     </row>
     <row r="279" spans="1:10" ht="56" x14ac:dyDescent="0.35">
       <c r="A279" s="9" t="str">
-        <f t="shared" ref="A279:A284" si="38">"02.10.2014"</f>
+        <f t="shared" ref="A279:A284" si="39">"02.10.2014"</f>
         <v>02.10.2014</v>
       </c>
       <c r="B279" s="13"/>
@@ -10615,7 +10640,7 @@
     </row>
     <row r="280" spans="1:10" ht="42" x14ac:dyDescent="0.35">
       <c r="A280" s="9" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>02.10.2014</v>
       </c>
       <c r="B280" s="13"/>
@@ -10638,7 +10663,7 @@
     </row>
     <row r="281" spans="1:10" ht="28" x14ac:dyDescent="0.35">
       <c r="A281" s="9" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>02.10.2014</v>
       </c>
       <c r="B281" s="13"/>
@@ -10661,7 +10686,7 @@
     </row>
     <row r="282" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A282" s="9" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>02.10.2014</v>
       </c>
       <c r="B282" s="13"/>
@@ -10684,7 +10709,7 @@
     </row>
     <row r="283" spans="1:10" ht="28" x14ac:dyDescent="0.35">
       <c r="A283" s="9" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>02.10.2014</v>
       </c>
       <c r="B283" s="13"/>
@@ -10707,7 +10732,7 @@
     </row>
     <row r="284" spans="1:10" ht="28" x14ac:dyDescent="0.35">
       <c r="A284" s="9" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>02.10.2014</v>
       </c>
       <c r="B284" s="13"/>
@@ -10887,7 +10912,7 @@
     </row>
     <row r="292" spans="1:10" ht="28" x14ac:dyDescent="0.35">
       <c r="A292" s="9" t="str">
-        <f t="shared" ref="A292:A304" si="39">"04.06.2013"</f>
+        <f t="shared" ref="A292:A304" si="40">"04.06.2013"</f>
         <v>04.06.2013</v>
       </c>
       <c r="B292" s="13"/>
@@ -10910,7 +10935,7 @@
     </row>
     <row r="293" spans="1:10" ht="42" x14ac:dyDescent="0.35">
       <c r="A293" s="9" t="str">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>04.06.2013</v>
       </c>
       <c r="B293" s="13"/>
@@ -10933,7 +10958,7 @@
     </row>
     <row r="294" spans="1:10" ht="28" x14ac:dyDescent="0.35">
       <c r="A294" s="9" t="str">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>04.06.2013</v>
       </c>
       <c r="B294" s="13"/>
@@ -10956,7 +10981,7 @@
     </row>
     <row r="295" spans="1:10" ht="28" x14ac:dyDescent="0.35">
       <c r="A295" s="9" t="str">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>04.06.2013</v>
       </c>
       <c r="B295" s="13"/>
@@ -10979,7 +11004,7 @@
     </row>
     <row r="296" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A296" s="9" t="str">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>04.06.2013</v>
       </c>
       <c r="B296" s="13"/>
@@ -11002,7 +11027,7 @@
     </row>
     <row r="297" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A297" s="9" t="str">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>04.06.2013</v>
       </c>
       <c r="B297" s="13"/>
@@ -11025,7 +11050,7 @@
     </row>
     <row r="298" spans="1:10" ht="42" x14ac:dyDescent="0.35">
       <c r="A298" s="9" t="str">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>04.06.2013</v>
       </c>
       <c r="B298" s="13"/>
@@ -11048,7 +11073,7 @@
     </row>
     <row r="299" spans="1:10" ht="28" x14ac:dyDescent="0.35">
       <c r="A299" s="9" t="str">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>04.06.2013</v>
       </c>
       <c r="B299" s="13"/>
@@ -11071,7 +11096,7 @@
     </row>
     <row r="300" spans="1:10" ht="42" x14ac:dyDescent="0.35">
       <c r="A300" s="9" t="str">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>04.06.2013</v>
       </c>
       <c r="B300" s="13"/>
@@ -11094,7 +11119,7 @@
     </row>
     <row r="301" spans="1:10" ht="28" x14ac:dyDescent="0.35">
       <c r="A301" s="9" t="str">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>04.06.2013</v>
       </c>
       <c r="B301" s="13"/>
@@ -11117,7 +11142,7 @@
     </row>
     <row r="302" spans="1:10" ht="28" x14ac:dyDescent="0.35">
       <c r="A302" s="9" t="str">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>04.06.2013</v>
       </c>
       <c r="B302" s="13"/>
@@ -11140,7 +11165,7 @@
     </row>
     <row r="303" spans="1:10" ht="28" x14ac:dyDescent="0.35">
       <c r="A303" s="9" t="str">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>04.06.2013</v>
       </c>
       <c r="B303" s="13"/>
@@ -11163,7 +11188,7 @@
     </row>
     <row r="304" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A304" s="9" t="str">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>04.06.2013</v>
       </c>
       <c r="B304" s="13"/>
@@ -11211,7 +11236,7 @@
     </row>
     <row r="306" spans="1:10" ht="28" x14ac:dyDescent="0.35">
       <c r="A306" s="9" t="str">
-        <f t="shared" ref="A306:A307" si="40">"28.11.2012"</f>
+        <f t="shared" ref="A306:A307" si="41">"28.11.2012"</f>
         <v>28.11.2012</v>
       </c>
       <c r="B306" s="13"/>
@@ -11234,7 +11259,7 @@
     </row>
     <row r="307" spans="1:10" ht="42" x14ac:dyDescent="0.35">
       <c r="A307" s="9" t="str">
-        <f t="shared" si="40"/>
+        <f t="shared" si="41"/>
         <v>28.11.2012</v>
       </c>
       <c r="B307" s="13"/>
@@ -11282,7 +11307,7 @@
     </row>
     <row r="309" spans="1:10" ht="28" x14ac:dyDescent="0.35">
       <c r="A309" s="9" t="str">
-        <f t="shared" ref="A309:A312" si="41">"25.09.2012"</f>
+        <f t="shared" ref="A309:A312" si="42">"25.09.2012"</f>
         <v>25.09.2012</v>
       </c>
       <c r="B309" s="13"/>
@@ -11305,7 +11330,7 @@
     </row>
     <row r="310" spans="1:10" ht="42" x14ac:dyDescent="0.35">
       <c r="A310" s="9" t="str">
-        <f t="shared" si="41"/>
+        <f t="shared" si="42"/>
         <v>25.09.2012</v>
       </c>
       <c r="B310" s="13"/>
@@ -11328,7 +11353,7 @@
     </row>
     <row r="311" spans="1:10" ht="28" x14ac:dyDescent="0.35">
       <c r="A311" s="9" t="str">
-        <f t="shared" si="41"/>
+        <f t="shared" si="42"/>
         <v>25.09.2012</v>
       </c>
       <c r="B311" s="13"/>
@@ -11351,7 +11376,7 @@
     </row>
     <row r="312" spans="1:10" ht="42" x14ac:dyDescent="0.35">
       <c r="A312" s="9" t="str">
-        <f t="shared" si="41"/>
+        <f t="shared" si="42"/>
         <v>25.09.2012</v>
       </c>
       <c r="B312" s="13"/>
@@ -11399,7 +11424,7 @@
     </row>
     <row r="314" spans="1:10" ht="28" x14ac:dyDescent="0.35">
       <c r="A314" s="9" t="str">
-        <f t="shared" ref="A314:A316" si="42">"09.07.2012"</f>
+        <f t="shared" ref="A314:A316" si="43">"09.07.2012"</f>
         <v>09.07.2012</v>
       </c>
       <c r="B314" s="13"/>
@@ -11422,7 +11447,7 @@
     </row>
     <row r="315" spans="1:10" ht="28" x14ac:dyDescent="0.35">
       <c r="A315" s="9" t="str">
-        <f t="shared" si="42"/>
+        <f t="shared" si="43"/>
         <v>09.07.2012</v>
       </c>
       <c r="B315" s="13"/>
@@ -11443,7 +11468,7 @@
     </row>
     <row r="316" spans="1:10" ht="28" x14ac:dyDescent="0.35">
       <c r="A316" s="9" t="str">
-        <f t="shared" si="42"/>
+        <f t="shared" si="43"/>
         <v>09.07.2012</v>
       </c>
       <c r="B316" s="13"/>
@@ -11558,7 +11583,7 @@
     </row>
     <row r="321" spans="1:10" ht="42" x14ac:dyDescent="0.35">
       <c r="A321" s="9" t="str">
-        <f t="shared" ref="A321:A327" si="43">"16.09.2011"</f>
+        <f t="shared" ref="A321:A327" si="44">"16.09.2011"</f>
         <v>16.09.2011</v>
       </c>
       <c r="B321" s="13"/>
@@ -11581,7 +11606,7 @@
     </row>
     <row r="322" spans="1:10" ht="28" x14ac:dyDescent="0.35">
       <c r="A322" s="9" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>16.09.2011</v>
       </c>
       <c r="B322" s="13"/>
@@ -11604,7 +11629,7 @@
     </row>
     <row r="323" spans="1:10" ht="28" x14ac:dyDescent="0.35">
       <c r="A323" s="9" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>16.09.2011</v>
       </c>
       <c r="B323" s="13"/>
@@ -11625,7 +11650,7 @@
     </row>
     <row r="324" spans="1:10" ht="42" x14ac:dyDescent="0.35">
       <c r="A324" s="9" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>16.09.2011</v>
       </c>
       <c r="B324" s="13"/>
@@ -11648,7 +11673,7 @@
     </row>
     <row r="325" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A325" s="9" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>16.09.2011</v>
       </c>
       <c r="B325" s="13"/>
@@ -11671,7 +11696,7 @@
     </row>
     <row r="326" spans="1:10" ht="28" x14ac:dyDescent="0.35">
       <c r="A326" s="9" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>16.09.2011</v>
       </c>
       <c r="B326" s="13"/>
@@ -11692,7 +11717,7 @@
     </row>
     <row r="327" spans="1:10" ht="56" x14ac:dyDescent="0.35">
       <c r="A327" s="9" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>16.09.2011</v>
       </c>
       <c r="B327" s="13"/>
@@ -11740,7 +11765,7 @@
     </row>
     <row r="329" spans="1:10" ht="28" x14ac:dyDescent="0.35">
       <c r="A329" s="9" t="str">
-        <f t="shared" ref="A329:A331" si="44">"21.07.2011"</f>
+        <f t="shared" ref="A329:A331" si="45">"21.07.2011"</f>
         <v>21.07.2011</v>
       </c>
       <c r="B329" s="13"/>
@@ -11763,7 +11788,7 @@
     </row>
     <row r="330" spans="1:10" ht="28" x14ac:dyDescent="0.35">
       <c r="A330" s="9" t="str">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v>21.07.2011</v>
       </c>
       <c r="B330" s="13"/>
@@ -11786,7 +11811,7 @@
     </row>
     <row r="331" spans="1:10" ht="28" x14ac:dyDescent="0.35">
       <c r="A331" s="9" t="str">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v>21.07.2011</v>
       </c>
       <c r="B331" s="13"/>
@@ -11834,7 +11859,7 @@
     </row>
     <row r="333" spans="1:10" ht="28" x14ac:dyDescent="0.35">
       <c r="A333" s="9" t="str">
-        <f t="shared" ref="A333:A340" si="45">"10.05.2011"</f>
+        <f t="shared" ref="A333:A340" si="46">"10.05.2011"</f>
         <v>10.05.2011</v>
       </c>
       <c r="B333" s="13"/>
@@ -11857,7 +11882,7 @@
     </row>
     <row r="334" spans="1:10" ht="28" x14ac:dyDescent="0.35">
       <c r="A334" s="9" t="str">
-        <f t="shared" si="45"/>
+        <f t="shared" si="46"/>
         <v>10.05.2011</v>
       </c>
       <c r="B334" s="13"/>
@@ -11880,7 +11905,7 @@
     </row>
     <row r="335" spans="1:10" ht="56" x14ac:dyDescent="0.35">
       <c r="A335" s="9" t="str">
-        <f t="shared" si="45"/>
+        <f t="shared" si="46"/>
         <v>10.05.2011</v>
       </c>
       <c r="B335" s="13"/>
@@ -11903,7 +11928,7 @@
     </row>
     <row r="336" spans="1:10" ht="28" x14ac:dyDescent="0.35">
       <c r="A336" s="9" t="str">
-        <f t="shared" si="45"/>
+        <f t="shared" si="46"/>
         <v>10.05.2011</v>
       </c>
       <c r="B336" s="13"/>
@@ -11926,7 +11951,7 @@
     </row>
     <row r="337" spans="1:10" ht="56" x14ac:dyDescent="0.35">
       <c r="A337" s="9" t="str">
-        <f t="shared" si="45"/>
+        <f t="shared" si="46"/>
         <v>10.05.2011</v>
       </c>
       <c r="B337" s="13"/>
@@ -11949,7 +11974,7 @@
     </row>
     <row r="338" spans="1:10" ht="28" x14ac:dyDescent="0.35">
       <c r="A338" s="9" t="str">
-        <f t="shared" si="45"/>
+        <f t="shared" si="46"/>
         <v>10.05.2011</v>
       </c>
       <c r="B338" s="13"/>
@@ -11972,7 +11997,7 @@
     </row>
     <row r="339" spans="1:10" ht="56" x14ac:dyDescent="0.35">
       <c r="A339" s="9" t="str">
-        <f t="shared" si="45"/>
+        <f t="shared" si="46"/>
         <v>10.05.2011</v>
       </c>
       <c r="B339" s="13"/>
@@ -11995,7 +12020,7 @@
     </row>
     <row r="340" spans="1:10" ht="28" x14ac:dyDescent="0.35">
       <c r="A340" s="9" t="str">
-        <f t="shared" si="45"/>
+        <f t="shared" si="46"/>
         <v>10.05.2011</v>
       </c>
       <c r="B340" s="13"/>
@@ -12043,7 +12068,7 @@
     </row>
     <row r="342" spans="1:10" ht="28" x14ac:dyDescent="0.35">
       <c r="A342" s="9" t="str">
-        <f t="shared" ref="A342:A345" si="46">"07.05.2011"</f>
+        <f t="shared" ref="A342:A345" si="47">"07.05.2011"</f>
         <v>07.05.2011</v>
       </c>
       <c r="B342" s="13"/>
@@ -12066,7 +12091,7 @@
     </row>
     <row r="343" spans="1:10" ht="28" x14ac:dyDescent="0.35">
       <c r="A343" s="9" t="str">
-        <f t="shared" si="46"/>
+        <f t="shared" si="47"/>
         <v>07.05.2011</v>
       </c>
       <c r="B343" s="13"/>
@@ -12087,7 +12112,7 @@
     </row>
     <row r="344" spans="1:10" ht="42" x14ac:dyDescent="0.35">
       <c r="A344" s="9" t="str">
-        <f t="shared" si="46"/>
+        <f t="shared" si="47"/>
         <v>07.05.2011</v>
       </c>
       <c r="B344" s="13"/>
@@ -12110,7 +12135,7 @@
     </row>
     <row r="345" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A345" s="9" t="str">
-        <f t="shared" si="46"/>
+        <f t="shared" si="47"/>
         <v>07.05.2011</v>
       </c>
       <c r="B345" s="13"/>
@@ -12249,7 +12274,7 @@
     </row>
     <row r="351" spans="1:10" ht="42" x14ac:dyDescent="0.35">
       <c r="A351" s="9" t="str">
-        <f t="shared" ref="A351:A360" si="47">"04.10.2010"</f>
+        <f t="shared" ref="A351:A360" si="48">"04.10.2010"</f>
         <v>04.10.2010</v>
       </c>
       <c r="B351" s="13"/>
@@ -12271,7 +12296,7 @@
     </row>
     <row r="352" spans="1:10" ht="42" x14ac:dyDescent="0.35">
       <c r="A352" s="9" t="str">
-        <f t="shared" si="47"/>
+        <f t="shared" si="48"/>
         <v>04.10.2010</v>
       </c>
       <c r="B352" s="13"/>
@@ -12293,7 +12318,7 @@
     </row>
     <row r="353" spans="1:10" ht="56" x14ac:dyDescent="0.35">
       <c r="A353" s="9" t="str">
-        <f t="shared" si="47"/>
+        <f t="shared" si="48"/>
         <v>04.10.2010</v>
       </c>
       <c r="B353" s="13"/>
@@ -12315,7 +12340,7 @@
     </row>
     <row r="354" spans="1:10" ht="42" x14ac:dyDescent="0.35">
       <c r="A354" s="9" t="str">
-        <f t="shared" si="47"/>
+        <f t="shared" si="48"/>
         <v>04.10.2010</v>
       </c>
       <c r="B354" s="13"/>
@@ -12338,7 +12363,7 @@
     </row>
     <row r="355" spans="1:10" ht="42" x14ac:dyDescent="0.35">
       <c r="A355" s="9" t="str">
-        <f t="shared" si="47"/>
+        <f t="shared" si="48"/>
         <v>04.10.2010</v>
       </c>
       <c r="B355" s="13"/>
@@ -12363,7 +12388,7 @@
     </row>
     <row r="356" spans="1:10" ht="28" x14ac:dyDescent="0.35">
       <c r="A356" s="9" t="str">
-        <f t="shared" si="47"/>
+        <f t="shared" si="48"/>
         <v>04.10.2010</v>
       </c>
       <c r="B356" s="13"/>
@@ -12388,7 +12413,7 @@
     </row>
     <row r="357" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A357" s="9" t="str">
-        <f t="shared" si="47"/>
+        <f t="shared" si="48"/>
         <v>04.10.2010</v>
       </c>
       <c r="B357" s="13"/>
@@ -12408,7 +12433,7 @@
     </row>
     <row r="358" spans="1:10" ht="42" x14ac:dyDescent="0.35">
       <c r="A358" s="9" t="str">
-        <f t="shared" si="47"/>
+        <f t="shared" si="48"/>
         <v>04.10.2010</v>
       </c>
       <c r="B358" s="13"/>
@@ -12433,7 +12458,7 @@
     </row>
     <row r="359" spans="1:10" ht="28" x14ac:dyDescent="0.35">
       <c r="A359" s="9" t="str">
-        <f t="shared" si="47"/>
+        <f t="shared" si="48"/>
         <v>04.10.2010</v>
       </c>
       <c r="B359" s="13"/>
@@ -12456,7 +12481,7 @@
     </row>
     <row r="360" spans="1:10" ht="28" x14ac:dyDescent="0.35">
       <c r="A360" s="9" t="str">
-        <f t="shared" si="47"/>
+        <f t="shared" si="48"/>
         <v>04.10.2010</v>
       </c>
       <c r="B360" s="13"/>
@@ -12506,7 +12531,7 @@
     </row>
     <row r="362" spans="1:10" ht="42" x14ac:dyDescent="0.35">
       <c r="A362" s="9" t="str">
-        <f t="shared" ref="A362:A367" si="48">"24.06.2010"</f>
+        <f t="shared" ref="A362:A367" si="49">"24.06.2010"</f>
         <v>24.06.2010</v>
       </c>
       <c r="B362" s="13"/>
@@ -12529,7 +12554,7 @@
     </row>
     <row r="363" spans="1:10" ht="28" x14ac:dyDescent="0.35">
       <c r="A363" s="9" t="str">
-        <f t="shared" si="48"/>
+        <f t="shared" si="49"/>
         <v>24.06.2010</v>
       </c>
       <c r="B363" s="13"/>
@@ -12552,7 +12577,7 @@
     </row>
     <row r="364" spans="1:10" ht="42" x14ac:dyDescent="0.35">
       <c r="A364" s="9" t="str">
-        <f t="shared" si="48"/>
+        <f t="shared" si="49"/>
         <v>24.06.2010</v>
       </c>
       <c r="B364" s="13"/>
@@ -12575,7 +12600,7 @@
     </row>
     <row r="365" spans="1:10" ht="28" x14ac:dyDescent="0.35">
       <c r="A365" s="9" t="str">
-        <f t="shared" si="48"/>
+        <f t="shared" si="49"/>
         <v>24.06.2010</v>
       </c>
       <c r="B365" s="13"/>
@@ -12598,7 +12623,7 @@
     </row>
     <row r="366" spans="1:10" ht="42" x14ac:dyDescent="0.35">
       <c r="A366" s="9" t="str">
-        <f t="shared" si="48"/>
+        <f t="shared" si="49"/>
         <v>24.06.2010</v>
       </c>
       <c r="B366" s="13"/>
@@ -12621,7 +12646,7 @@
     </row>
     <row r="367" spans="1:10" ht="28" x14ac:dyDescent="0.35">
       <c r="A367" s="9" t="str">
-        <f t="shared" si="48"/>
+        <f t="shared" si="49"/>
         <v>24.06.2010</v>
       </c>
       <c r="B367" s="13"/>
@@ -12719,7 +12744,7 @@
     </row>
     <row r="371" spans="1:10" ht="42" x14ac:dyDescent="0.35">
       <c r="A371" s="9" t="str">
-        <f t="shared" ref="A371:A376" si="49">"12.03.2010"</f>
+        <f t="shared" ref="A371:A376" si="50">"12.03.2010"</f>
         <v>12.03.2010</v>
       </c>
       <c r="B371" s="13"/>
@@ -12742,7 +12767,7 @@
     </row>
     <row r="372" spans="1:10" ht="28" x14ac:dyDescent="0.35">
       <c r="A372" s="9" t="str">
-        <f t="shared" si="49"/>
+        <f t="shared" si="50"/>
         <v>12.03.2010</v>
       </c>
       <c r="B372" s="13"/>
@@ -12765,7 +12790,7 @@
     </row>
     <row r="373" spans="1:10" ht="28" x14ac:dyDescent="0.35">
       <c r="A373" s="9" t="str">
-        <f t="shared" si="49"/>
+        <f t="shared" si="50"/>
         <v>12.03.2010</v>
       </c>
       <c r="B373" s="13"/>
@@ -12788,7 +12813,7 @@
     </row>
     <row r="374" spans="1:10" ht="42" x14ac:dyDescent="0.35">
       <c r="A374" s="9" t="str">
-        <f t="shared" si="49"/>
+        <f t="shared" si="50"/>
         <v>12.03.2010</v>
       </c>
       <c r="B374" s="13"/>
@@ -12811,7 +12836,7 @@
     </row>
     <row r="375" spans="1:10" ht="42" x14ac:dyDescent="0.35">
       <c r="A375" s="9" t="str">
-        <f t="shared" si="49"/>
+        <f t="shared" si="50"/>
         <v>12.03.2010</v>
       </c>
       <c r="B375" s="13"/>
@@ -12834,7 +12859,7 @@
     </row>
     <row r="376" spans="1:10" ht="42" x14ac:dyDescent="0.35">
       <c r="A376" s="9" t="str">
-        <f t="shared" si="49"/>
+        <f t="shared" si="50"/>
         <v>12.03.2010</v>
       </c>
       <c r="B376" s="13"/>

</xml_diff>

<commit_message>
added recording of webinar 19th March 2025
</commit_message>
<xml_diff>
--- a/data/seminars.xlsx
+++ b/data/seminars.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\rufibach\90_github_repos\BBS\home\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09807DD3-E417-4DF8-93FA-1A98BC47EE48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01270939-DE68-4EDC-B7CD-78E6BF6DF0C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1723" uniqueCount="1387">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1724" uniqueCount="1388">
   <si>
     <t>Anja Schiel</t>
   </si>
@@ -4193,6 +4193,9 @@
   </si>
   <si>
     <t>event</t>
+  </si>
+  <si>
+    <t>https://youtu.be/OC-zPB-SJrc</t>
   </si>
 </sst>
 </file>
@@ -4713,9 +4716,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L1100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A461" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F416" sqref="F416"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4780,7 +4783,9 @@
       <c r="B2" s="3" t="s">
         <v>1377</v>
       </c>
-      <c r="C2" s="4"/>
+      <c r="C2" s="4" t="s">
+        <v>1387</v>
+      </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>

</xml_diff>

<commit_message>
added Mats's deck (30-Oct-2025)
</commit_message>
<xml_diff>
--- a/data/seminars.xlsx
+++ b/data/seminars.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\schaej17\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28FC6D56-40E5-4981-8A8E-E2005E9707F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D59CA46-63E3-4BF1-862C-4DB0F2030961}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="13776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3480" yWindow="3720" windowWidth="17280" windowHeight="9960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Conferences" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1795" uniqueCount="1433">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1796" uniqueCount="1434">
   <si>
     <t>Anja Schiel</t>
   </si>
@@ -4331,6 +4331,9 @@
   </si>
   <si>
     <t>20251030_6_Didelez.pdf</t>
+  </si>
+  <si>
+    <t>20251030_1_Stensrud.pdf</t>
   </si>
 </sst>
 </file>
@@ -5044,7 +5047,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="K1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K4" sqref="K4"/>
+      <selection pane="bottomLeft" activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5101,7 +5104,7 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="str">
-        <f>"30.10.2025"</f>
+        <f t="shared" ref="A2:A7" si="0">"30.10.2025"</f>
         <v>30.10.2025</v>
       </c>
       <c r="B2" s="3" t="s">
@@ -5123,11 +5126,13 @@
       <c r="J2" s="13" t="s">
         <v>1422</v>
       </c>
-      <c r="K2" s="2"/>
+      <c r="K2" s="2" t="s">
+        <v>1433</v>
+      </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="str">
-        <f>"30.10.2025"</f>
+        <f t="shared" si="0"/>
         <v>30.10.2025</v>
       </c>
       <c r="B3" s="3" t="s">
@@ -5155,7 +5160,7 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="str">
-        <f>"30.10.2025"</f>
+        <f t="shared" si="0"/>
         <v>30.10.2025</v>
       </c>
       <c r="B4" s="3" t="s">
@@ -5183,7 +5188,7 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="str">
-        <f>"30.10.2025"</f>
+        <f t="shared" si="0"/>
         <v>30.10.2025</v>
       </c>
       <c r="B5" s="3" t="s">
@@ -5211,7 +5216,7 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="str">
-        <f>"30.10.2025"</f>
+        <f t="shared" si="0"/>
         <v>30.10.2025</v>
       </c>
       <c r="B6" s="3" t="s">
@@ -5239,7 +5244,7 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="str">
-        <f>"30.10.2025"</f>
+        <f t="shared" si="0"/>
         <v>30.10.2025</v>
       </c>
       <c r="B7" s="32" t="s">
@@ -5521,7 +5526,7 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="str">
-        <f t="shared" ref="A17:A18" si="0">"19.03.2025"</f>
+        <f t="shared" ref="A17:A18" si="1">"19.03.2025"</f>
         <v>19.03.2025</v>
       </c>
       <c r="B17" s="3" t="s">
@@ -5549,7 +5554,7 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>19.03.2025</v>
       </c>
       <c r="B18" s="3" t="s">
@@ -5625,7 +5630,7 @@
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="str">
-        <f t="shared" ref="A21:A29" si="1">"25.09.2024"</f>
+        <f t="shared" ref="A21:A29" si="2">"25.09.2024"</f>
         <v>25.09.2024</v>
       </c>
       <c r="B21" s="3" t="s">
@@ -5657,7 +5662,7 @@
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>25.09.2024</v>
       </c>
       <c r="B22" s="3" t="s">
@@ -5685,7 +5690,7 @@
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" s="5" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>25.09.2024</v>
       </c>
       <c r="B23" s="3" t="s">
@@ -5713,7 +5718,7 @@
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>25.09.2024</v>
       </c>
       <c r="B24" s="3" t="s">
@@ -5741,7 +5746,7 @@
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" s="5" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>25.09.2024</v>
       </c>
       <c r="B25" s="3" t="s">
@@ -5769,7 +5774,7 @@
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" s="5" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>25.09.2024</v>
       </c>
       <c r="B26" s="3" t="s">
@@ -5797,7 +5802,7 @@
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" s="5" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>25.09.2024</v>
       </c>
       <c r="B27" s="3" t="s">
@@ -5825,7 +5830,7 @@
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28" s="5" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>25.09.2024</v>
       </c>
       <c r="B28" s="3" t="s">
@@ -5853,7 +5858,7 @@
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" s="5" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>25.09.2024</v>
       </c>
       <c r="B29" s="3" t="s">
@@ -5899,7 +5904,7 @@
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31" s="5" t="str">
-        <f t="shared" ref="A31:A37" si="2">"29.08.2024"</f>
+        <f t="shared" ref="A31:A37" si="3">"29.08.2024"</f>
         <v>29.08.2024</v>
       </c>
       <c r="B31" s="3" t="s">
@@ -5931,7 +5936,7 @@
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32" s="5" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>29.08.2024</v>
       </c>
       <c r="B32" s="3" t="s">
@@ -5959,7 +5964,7 @@
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A33" s="5" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>29.08.2024</v>
       </c>
       <c r="B33" s="3" t="s">
@@ -5987,7 +5992,7 @@
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A34" s="5" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>29.08.2024</v>
       </c>
       <c r="B34" s="3" t="s">
@@ -6015,7 +6020,7 @@
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A35" s="5" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>29.08.2024</v>
       </c>
       <c r="B35" s="3" t="s">
@@ -6043,7 +6048,7 @@
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A36" s="5" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>29.08.2024</v>
       </c>
       <c r="B36" s="3" t="s">
@@ -6071,7 +6076,7 @@
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A37" s="5" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>29.08.2024</v>
       </c>
       <c r="B37" s="3" t="s">
@@ -6099,7 +6104,7 @@
     </row>
     <row r="38" spans="1:12" ht="18" x14ac:dyDescent="0.35">
       <c r="A38" s="5" t="str">
-        <f t="shared" ref="A38:A43" si="3">"16.05.2024"</f>
+        <f t="shared" ref="A38:A43" si="4">"16.05.2024"</f>
         <v>16.05.2024</v>
       </c>
       <c r="B38" s="3" t="s">
@@ -6127,7 +6132,7 @@
     </row>
     <row r="39" spans="1:12" ht="18" x14ac:dyDescent="0.35">
       <c r="A39" s="5" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>16.05.2024</v>
       </c>
       <c r="B39" s="3" t="s">
@@ -6155,7 +6160,7 @@
     </row>
     <row r="40" spans="1:12" ht="18" x14ac:dyDescent="0.35">
       <c r="A40" s="5" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>16.05.2024</v>
       </c>
       <c r="B40" s="3" t="s">
@@ -6183,7 +6188,7 @@
     </row>
     <row r="41" spans="1:12" ht="18" x14ac:dyDescent="0.35">
       <c r="A41" s="5" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>16.05.2024</v>
       </c>
       <c r="B41" s="3" t="s">
@@ -6211,7 +6216,7 @@
     </row>
     <row r="42" spans="1:12" ht="18" x14ac:dyDescent="0.35">
       <c r="A42" s="5" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>16.05.2024</v>
       </c>
       <c r="B42" s="3" t="s">
@@ -6239,7 +6244,7 @@
     </row>
     <row r="43" spans="1:12" ht="18" x14ac:dyDescent="0.35">
       <c r="A43" s="5" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>16.05.2024</v>
       </c>
       <c r="B43" s="3" t="s">
@@ -6267,7 +6272,7 @@
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A44" s="5" t="str">
-        <f t="shared" ref="A44:A48" si="4">"16.05.2024"</f>
+        <f t="shared" ref="A44:A48" si="5">"16.05.2024"</f>
         <v>16.05.2024</v>
       </c>
       <c r="B44" s="3" t="s">
@@ -6295,7 +6300,7 @@
     </row>
     <row r="45" spans="1:12" ht="18" x14ac:dyDescent="0.35">
       <c r="A45" s="5" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>16.05.2024</v>
       </c>
       <c r="B45" s="3" t="s">
@@ -6324,7 +6329,7 @@
     </row>
     <row r="46" spans="1:12" ht="18" x14ac:dyDescent="0.35">
       <c r="A46" s="5" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>16.05.2024</v>
       </c>
       <c r="B46" s="3" t="s">
@@ -6352,7 +6357,7 @@
     </row>
     <row r="47" spans="1:12" ht="18" x14ac:dyDescent="0.35">
       <c r="A47" s="5" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>16.05.2024</v>
       </c>
       <c r="B47" s="3" t="s">
@@ -6380,7 +6385,7 @@
     </row>
     <row r="48" spans="1:12" ht="18" x14ac:dyDescent="0.35">
       <c r="A48" s="5" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>16.05.2024</v>
       </c>
       <c r="B48" s="3" t="s">
@@ -6616,7 +6621,7 @@
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A57" s="5" t="str">
-        <f t="shared" ref="A57:A64" si="5">"06.11.2023"</f>
+        <f t="shared" ref="A57:A64" si="6">"06.11.2023"</f>
         <v>06.11.2023</v>
       </c>
       <c r="B57" s="3" t="s">
@@ -6648,7 +6653,7 @@
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A58" s="5" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>06.11.2023</v>
       </c>
       <c r="B58" s="3" t="s">
@@ -6676,7 +6681,7 @@
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A59" s="5" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>06.11.2023</v>
       </c>
       <c r="B59" s="3" t="s">
@@ -6704,7 +6709,7 @@
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A60" s="5" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>06.11.2023</v>
       </c>
       <c r="B60" s="3" t="s">
@@ -6732,7 +6737,7 @@
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A61" s="5" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>06.11.2023</v>
       </c>
       <c r="B61" s="3" t="s">
@@ -6760,7 +6765,7 @@
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A62" s="5" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>06.11.2023</v>
       </c>
       <c r="B62" s="3" t="s">
@@ -6788,7 +6793,7 @@
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A63" s="5" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>06.11.2023</v>
       </c>
       <c r="B63" s="3" t="s">
@@ -6816,7 +6821,7 @@
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A64" s="5" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>06.11.2023</v>
       </c>
       <c r="B64" s="3" t="s">
@@ -6842,7 +6847,7 @@
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A65" s="5" t="str">
-        <f t="shared" ref="A65:A71" si="6">"16.10.2023"</f>
+        <f t="shared" ref="A65:A71" si="7">"16.10.2023"</f>
         <v>16.10.2023</v>
       </c>
       <c r="B65" s="3" t="s">
@@ -6870,7 +6875,7 @@
     </row>
     <row r="66" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A66" s="5" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>16.10.2023</v>
       </c>
       <c r="B66" s="3" t="s">
@@ -6898,7 +6903,7 @@
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A67" s="5" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>16.10.2023</v>
       </c>
       <c r="B67" s="3" t="s">
@@ -6926,7 +6931,7 @@
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A68" s="5" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>16.10.2023</v>
       </c>
       <c r="B68" s="3" t="s">
@@ -6954,7 +6959,7 @@
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A69" s="5" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>16.10.2023</v>
       </c>
       <c r="B69" s="3" t="s">
@@ -6982,7 +6987,7 @@
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A70" s="5" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>16.10.2023</v>
       </c>
       <c r="B70" s="3" t="s">
@@ -7010,7 +7015,7 @@
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A71" s="5" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>16.10.2023</v>
       </c>
       <c r="B71" s="3" t="s">
@@ -7038,7 +7043,7 @@
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A72" s="5" t="str">
-        <f t="shared" ref="A72:A77" si="7">"04.10.2023"</f>
+        <f t="shared" ref="A72:A77" si="8">"04.10.2023"</f>
         <v>04.10.2023</v>
       </c>
       <c r="B72" s="3" t="s">
@@ -7066,7 +7071,7 @@
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A73" s="5" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>04.10.2023</v>
       </c>
       <c r="B73" s="3" t="s">
@@ -7094,7 +7099,7 @@
     </row>
     <row r="74" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A74" s="5" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>04.10.2023</v>
       </c>
       <c r="B74" s="3" t="s">
@@ -7122,7 +7127,7 @@
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A75" s="5" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>04.10.2023</v>
       </c>
       <c r="B75" s="3" t="s">
@@ -7150,7 +7155,7 @@
     </row>
     <row r="76" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A76" s="5" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>04.10.2023</v>
       </c>
       <c r="B76" s="3" t="s">
@@ -7178,7 +7183,7 @@
     </row>
     <row r="77" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A77" s="5" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>04.10.2023</v>
       </c>
       <c r="B77" s="3" t="s">
@@ -7252,7 +7257,7 @@
     </row>
     <row r="80" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A80" s="5" t="str">
-        <f t="shared" ref="A80:A84" si="8">"21.06.2023"</f>
+        <f t="shared" ref="A80:A84" si="9">"21.06.2023"</f>
         <v>21.06.2023</v>
       </c>
       <c r="B80" s="3" t="s">
@@ -7280,7 +7285,7 @@
     </row>
     <row r="81" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A81" s="5" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>21.06.2023</v>
       </c>
       <c r="B81" s="3" t="s">
@@ -7308,7 +7313,7 @@
     </row>
     <row r="82" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A82" s="5" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>21.06.2023</v>
       </c>
       <c r="B82" s="3" t="s">
@@ -7336,7 +7341,7 @@
     </row>
     <row r="83" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A83" s="5" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>21.06.2023</v>
       </c>
       <c r="B83" s="3" t="s">
@@ -7364,7 +7369,7 @@
     </row>
     <row r="84" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A84" s="5" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>21.06.2023</v>
       </c>
       <c r="B84" s="3" t="s">
@@ -7524,7 +7529,7 @@
     </row>
     <row r="90" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A90" s="1" t="str">
-        <f t="shared" ref="A90:A96" si="9">"15.03.2023"</f>
+        <f t="shared" ref="A90:A96" si="10">"15.03.2023"</f>
         <v>15.03.2023</v>
       </c>
       <c r="B90" s="3" t="s">
@@ -7554,7 +7559,7 @@
     </row>
     <row r="91" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A91" s="1" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>15.03.2023</v>
       </c>
       <c r="B91" s="3" t="s">
@@ -7582,7 +7587,7 @@
     </row>
     <row r="92" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A92" s="1" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>15.03.2023</v>
       </c>
       <c r="B92" s="3" t="s">
@@ -7610,7 +7615,7 @@
     </row>
     <row r="93" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A93" s="1" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>15.03.2023</v>
       </c>
       <c r="B93" s="3" t="s">
@@ -7638,7 +7643,7 @@
     </row>
     <row r="94" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A94" s="1" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>15.03.2023</v>
       </c>
       <c r="B94" s="3" t="s">
@@ -7666,7 +7671,7 @@
     </row>
     <row r="95" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A95" s="1" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>15.03.2023</v>
       </c>
       <c r="B95" s="3" t="s">
@@ -7694,7 +7699,7 @@
     </row>
     <row r="96" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A96" s="1" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>15.03.2023</v>
       </c>
       <c r="B96" s="3" t="s">
@@ -7754,7 +7759,7 @@
     </row>
     <row r="98" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A98" s="5" t="str">
-        <f t="shared" ref="A98:A103" si="10">"15.12.2022"</f>
+        <f t="shared" ref="A98:A103" si="11">"15.12.2022"</f>
         <v>15.12.2022</v>
       </c>
       <c r="B98" s="3" t="s">
@@ -7782,7 +7787,7 @@
     </row>
     <row r="99" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A99" s="5" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>15.12.2022</v>
       </c>
       <c r="B99" s="3" t="s">
@@ -7810,7 +7815,7 @@
     </row>
     <row r="100" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A100" s="5" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>15.12.2022</v>
       </c>
       <c r="B100" s="3" t="s">
@@ -7838,7 +7843,7 @@
     </row>
     <row r="101" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A101" s="5" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>15.12.2022</v>
       </c>
       <c r="B101" s="3" t="s">
@@ -7866,7 +7871,7 @@
     </row>
     <row r="102" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A102" s="5" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>15.12.2022</v>
       </c>
       <c r="B102" s="3" t="s">
@@ -7894,7 +7899,7 @@
     </row>
     <row r="103" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A103" s="5" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>15.12.2022</v>
       </c>
       <c r="B103" s="3" t="s">
@@ -7920,7 +7925,7 @@
     </row>
     <row r="104" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A104" s="5" t="str">
-        <f t="shared" ref="A104:A109" si="11">"08.12.2022"</f>
+        <f t="shared" ref="A104:A109" si="12">"08.12.2022"</f>
         <v>08.12.2022</v>
       </c>
       <c r="B104" s="3" t="s">
@@ -7952,7 +7957,7 @@
     </row>
     <row r="105" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A105" s="5" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>08.12.2022</v>
       </c>
       <c r="B105" s="3" t="s">
@@ -7980,7 +7985,7 @@
     </row>
     <row r="106" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A106" s="5" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>08.12.2022</v>
       </c>
       <c r="B106" s="3" t="s">
@@ -8008,7 +8013,7 @@
     </row>
     <row r="107" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A107" s="5" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>08.12.2022</v>
       </c>
       <c r="B107" s="3" t="s">
@@ -8037,7 +8042,7 @@
     </row>
     <row r="108" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A108" s="5" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>08.12.2022</v>
       </c>
       <c r="B108" s="3" t="s">
@@ -8065,7 +8070,7 @@
     </row>
     <row r="109" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A109" s="5" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>08.12.2022</v>
       </c>
       <c r="B109" s="3" t="s">
@@ -8147,7 +8152,7 @@
     </row>
     <row r="112" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A112" s="5" t="str">
-        <f t="shared" ref="A112:A114" si="12">"30.11.2022"</f>
+        <f t="shared" ref="A112:A114" si="13">"30.11.2022"</f>
         <v>30.11.2022</v>
       </c>
       <c r="B112" s="3" t="s">
@@ -8173,7 +8178,7 @@
     </row>
     <row r="113" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A113" s="5" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>30.11.2022</v>
       </c>
       <c r="B113" s="3" t="s">
@@ -8199,7 +8204,7 @@
     </row>
     <row r="114" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A114" s="5" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>30.11.2022</v>
       </c>
       <c r="B114" s="3" t="s">
@@ -8225,7 +8230,7 @@
     </row>
     <row r="115" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A115" s="17" t="str">
-        <f t="shared" ref="A115:A120" si="13">"15.07.2022"</f>
+        <f t="shared" ref="A115:A120" si="14">"15.07.2022"</f>
         <v>15.07.2022</v>
       </c>
       <c r="B115" s="14" t="s">
@@ -8255,7 +8260,7 @@
     </row>
     <row r="116" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A116" s="17" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>15.07.2022</v>
       </c>
       <c r="B116" s="14" t="s">
@@ -8283,7 +8288,7 @@
     </row>
     <row r="117" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A117" s="17" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>15.07.2022</v>
       </c>
       <c r="B117" s="14" t="s">
@@ -8311,7 +8316,7 @@
     </row>
     <row r="118" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A118" s="17" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>15.07.2022</v>
       </c>
       <c r="B118" s="14" t="s">
@@ -8339,7 +8344,7 @@
     </row>
     <row r="119" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A119" s="17" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>15.07.2022</v>
       </c>
       <c r="B119" s="14" t="s">
@@ -8367,7 +8372,7 @@
     </row>
     <row r="120" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A120" s="17" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>15.07.2022</v>
       </c>
       <c r="B120" s="14" t="s">
@@ -8419,7 +8424,7 @@
     </row>
     <row r="122" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A122" s="17" t="str">
-        <f t="shared" ref="A122:A128" si="14">"23.06.2022"</f>
+        <f t="shared" ref="A122:A128" si="15">"23.06.2022"</f>
         <v>23.06.2022</v>
       </c>
       <c r="B122" s="3" t="s">
@@ -8445,7 +8450,7 @@
     </row>
     <row r="123" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A123" s="17" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>23.06.2022</v>
       </c>
       <c r="B123" s="3" t="s">
@@ -8473,7 +8478,7 @@
     </row>
     <row r="124" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A124" s="17" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>23.06.2022</v>
       </c>
       <c r="B124" s="3" t="s">
@@ -8501,7 +8506,7 @@
     </row>
     <row r="125" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A125" s="17" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>23.06.2022</v>
       </c>
       <c r="B125" s="3" t="s">
@@ -8529,7 +8534,7 @@
     </row>
     <row r="126" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A126" s="17" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>23.06.2022</v>
       </c>
       <c r="B126" s="3" t="s">
@@ -8557,7 +8562,7 @@
     </row>
     <row r="127" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A127" s="17" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>23.06.2022</v>
       </c>
       <c r="B127" s="3" t="s">
@@ -8585,7 +8590,7 @@
     </row>
     <row r="128" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A128" s="17" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>23.06.2022</v>
       </c>
       <c r="B128" s="3" t="s">
@@ -8751,7 +8756,7 @@
     </row>
     <row r="134" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A134" s="5" t="str">
-        <f t="shared" ref="A134:A136" si="15">"21.02.2022"</f>
+        <f t="shared" ref="A134:A136" si="16">"21.02.2022"</f>
         <v>21.02.2022</v>
       </c>
       <c r="B134" s="3"/>
@@ -8777,7 +8782,7 @@
     </row>
     <row r="135" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A135" s="5" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>21.02.2022</v>
       </c>
       <c r="B135" s="3"/>
@@ -8803,7 +8808,7 @@
     </row>
     <row r="136" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A136" s="5" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>21.02.2022</v>
       </c>
       <c r="B136" s="3"/>
@@ -8857,7 +8862,7 @@
     </row>
     <row r="138" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A138" s="9" t="str">
-        <f t="shared" ref="A138:A141" si="16">"27.07.2021"</f>
+        <f t="shared" ref="A138:A141" si="17">"27.07.2021"</f>
         <v>27.07.2021</v>
       </c>
       <c r="B138" s="12"/>
@@ -8883,7 +8888,7 @@
     </row>
     <row r="139" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A139" s="9" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>27.07.2021</v>
       </c>
       <c r="B139" s="12"/>
@@ -8909,7 +8914,7 @@
     </row>
     <row r="140" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A140" s="9" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>27.07.2021</v>
       </c>
       <c r="B140" s="12"/>
@@ -8935,7 +8940,7 @@
     </row>
     <row r="141" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A141" s="9" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>27.07.2021</v>
       </c>
       <c r="B141" s="12"/>
@@ -8991,7 +8996,7 @@
     </row>
     <row r="143" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A143" s="9" t="str">
-        <f t="shared" ref="A143:A149" si="17">"28.06.2021"</f>
+        <f t="shared" ref="A143:A149" si="18">"28.06.2021"</f>
         <v>28.06.2021</v>
       </c>
       <c r="B143" s="12"/>
@@ -9017,7 +9022,7 @@
     </row>
     <row r="144" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A144" s="9" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>28.06.2021</v>
       </c>
       <c r="B144" s="12"/>
@@ -9043,7 +9048,7 @@
     </row>
     <row r="145" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A145" s="9" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>28.06.2021</v>
       </c>
       <c r="B145" s="12"/>
@@ -9069,7 +9074,7 @@
     </row>
     <row r="146" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A146" s="9" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>28.06.2021</v>
       </c>
       <c r="B146" s="12"/>
@@ -9095,7 +9100,7 @@
     </row>
     <row r="147" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A147" s="9" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>28.06.2021</v>
       </c>
       <c r="B147" s="12"/>
@@ -9121,7 +9126,7 @@
     </row>
     <row r="148" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A148" s="9" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>28.06.2021</v>
       </c>
       <c r="B148" s="12"/>
@@ -9147,7 +9152,7 @@
     </row>
     <row r="149" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A149" s="9" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>28.06.2021</v>
       </c>
       <c r="B149" s="12"/>
@@ -9203,7 +9208,7 @@
     </row>
     <row r="151" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A151" s="9" t="str">
-        <f t="shared" ref="A151:A153" si="18">"16.06.2021"</f>
+        <f t="shared" ref="A151:A153" si="19">"16.06.2021"</f>
         <v>16.06.2021</v>
       </c>
       <c r="B151" s="12"/>
@@ -9229,7 +9234,7 @@
     </row>
     <row r="152" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A152" s="9" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>16.06.2021</v>
       </c>
       <c r="B152" s="12"/>
@@ -9255,7 +9260,7 @@
     </row>
     <row r="153" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A153" s="9" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>16.06.2021</v>
       </c>
       <c r="B153" s="12"/>
@@ -9311,7 +9316,7 @@
     </row>
     <row r="155" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A155" s="9" t="str">
-        <f t="shared" ref="A155:A163" si="19">"22.03.2021"</f>
+        <f t="shared" ref="A155:A163" si="20">"22.03.2021"</f>
         <v>22.03.2021</v>
       </c>
       <c r="B155" s="12"/>
@@ -9337,7 +9342,7 @@
     </row>
     <row r="156" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A156" s="9" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>22.03.2021</v>
       </c>
       <c r="B156" s="12"/>
@@ -9363,7 +9368,7 @@
     </row>
     <row r="157" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A157" s="9" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>22.03.2021</v>
       </c>
       <c r="B157" s="12"/>
@@ -9389,7 +9394,7 @@
     </row>
     <row r="158" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A158" s="9" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>22.03.2021</v>
       </c>
       <c r="B158" s="12"/>
@@ -9415,7 +9420,7 @@
     </row>
     <row r="159" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A159" s="9" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>22.03.2021</v>
       </c>
       <c r="B159" s="12"/>
@@ -9441,7 +9446,7 @@
     </row>
     <row r="160" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A160" s="9" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>22.03.2021</v>
       </c>
       <c r="B160" s="12"/>
@@ -9467,7 +9472,7 @@
     </row>
     <row r="161" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A161" s="9" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>22.03.2021</v>
       </c>
       <c r="B161" s="12"/>
@@ -9493,7 +9498,7 @@
     </row>
     <row r="162" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A162" s="9" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>22.03.2021</v>
       </c>
       <c r="B162" s="12"/>
@@ -9519,7 +9524,7 @@
     </row>
     <row r="163" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A163" s="9" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>22.03.2021</v>
       </c>
       <c r="B163" s="12"/>
@@ -9573,7 +9578,7 @@
     </row>
     <row r="165" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A165" s="9" t="str">
-        <f t="shared" ref="A165:A170" si="20">"08.03.2021"</f>
+        <f t="shared" ref="A165:A170" si="21">"08.03.2021"</f>
         <v>08.03.2021</v>
       </c>
       <c r="B165" s="12"/>
@@ -9599,7 +9604,7 @@
     </row>
     <row r="166" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A166" s="9" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>08.03.2021</v>
       </c>
       <c r="B166" s="12"/>
@@ -9625,7 +9630,7 @@
     </row>
     <row r="167" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A167" s="9" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>08.03.2021</v>
       </c>
       <c r="B167" s="12"/>
@@ -9651,7 +9656,7 @@
     </row>
     <row r="168" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A168" s="9" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>08.03.2021</v>
       </c>
       <c r="B168" s="12"/>
@@ -9677,7 +9682,7 @@
     </row>
     <row r="169" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A169" s="9" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>08.03.2021</v>
       </c>
       <c r="B169" s="12"/>
@@ -9703,7 +9708,7 @@
     </row>
     <row r="170" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A170" s="9" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>08.03.2021</v>
       </c>
       <c r="B170" s="12"/>
@@ -9757,7 +9762,7 @@
     </row>
     <row r="172" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A172" s="9" t="str">
-        <f t="shared" ref="A172:A178" si="21">"03.11.2020"</f>
+        <f t="shared" ref="A172:A178" si="22">"03.11.2020"</f>
         <v>03.11.2020</v>
       </c>
       <c r="B172" s="12"/>
@@ -9783,7 +9788,7 @@
     </row>
     <row r="173" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A173" s="9" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>03.11.2020</v>
       </c>
       <c r="B173" s="12"/>
@@ -9809,7 +9814,7 @@
     </row>
     <row r="174" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A174" s="9" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>03.11.2020</v>
       </c>
       <c r="B174" s="12"/>
@@ -9835,7 +9840,7 @@
     </row>
     <row r="175" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A175" s="9" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>03.11.2020</v>
       </c>
       <c r="B175" s="12"/>
@@ -9861,7 +9866,7 @@
     </row>
     <row r="176" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A176" s="9" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>03.11.2020</v>
       </c>
       <c r="B176" s="12"/>
@@ -9887,7 +9892,7 @@
     </row>
     <row r="177" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A177" s="9" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>03.11.2020</v>
       </c>
       <c r="B177" s="12"/>
@@ -9913,7 +9918,7 @@
     </row>
     <row r="178" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A178" s="9" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>03.11.2020</v>
       </c>
       <c r="B178" s="12"/>
@@ -9969,7 +9974,7 @@
     </row>
     <row r="180" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A180" s="9" t="str">
-        <f t="shared" ref="A180:A188" si="22">"07.09.2020"</f>
+        <f t="shared" ref="A180:A188" si="23">"07.09.2020"</f>
         <v>07.09.2020</v>
       </c>
       <c r="B180" s="12"/>
@@ -9995,7 +10000,7 @@
     </row>
     <row r="181" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A181" s="9" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>07.09.2020</v>
       </c>
       <c r="B181" s="12"/>
@@ -10021,7 +10026,7 @@
     </row>
     <row r="182" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A182" s="9" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>07.09.2020</v>
       </c>
       <c r="B182" s="12"/>
@@ -10047,7 +10052,7 @@
     </row>
     <row r="183" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A183" s="9" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>07.09.2020</v>
       </c>
       <c r="B183" s="12"/>
@@ -10073,7 +10078,7 @@
     </row>
     <row r="184" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A184" s="9" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>07.09.2020</v>
       </c>
       <c r="B184" s="12"/>
@@ -10099,7 +10104,7 @@
     </row>
     <row r="185" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A185" s="9" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>07.09.2020</v>
       </c>
       <c r="B185" s="12"/>
@@ -10125,7 +10130,7 @@
     </row>
     <row r="186" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A186" s="9" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>07.09.2020</v>
       </c>
       <c r="B186" s="12"/>
@@ -10151,7 +10156,7 @@
     </row>
     <row r="187" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A187" s="9" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>07.09.2020</v>
       </c>
       <c r="B187" s="12"/>
@@ -10177,7 +10182,7 @@
     </row>
     <row r="188" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A188" s="9" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>07.09.2020</v>
       </c>
       <c r="B188" s="12"/>
@@ -10231,7 +10236,7 @@
     </row>
     <row r="190" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A190" s="9" t="str">
-        <f t="shared" ref="A190:A193" si="23">"30.06.2020"</f>
+        <f t="shared" ref="A190:A193" si="24">"30.06.2020"</f>
         <v>30.06.2020</v>
       </c>
       <c r="B190" s="12"/>
@@ -10257,7 +10262,7 @@
     </row>
     <row r="191" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A191" s="9" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>30.06.2020</v>
       </c>
       <c r="B191" s="12"/>
@@ -10283,7 +10288,7 @@
     </row>
     <row r="192" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A192" s="9" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>30.06.2020</v>
       </c>
       <c r="B192" s="12"/>
@@ -10309,7 +10314,7 @@
     </row>
     <row r="193" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A193" s="9" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>30.06.2020</v>
       </c>
       <c r="B193" s="12"/>
@@ -10365,7 +10370,7 @@
     </row>
     <row r="195" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A195" s="9" t="str">
-        <f t="shared" ref="A195:A200" si="24">"29.06.2020"</f>
+        <f t="shared" ref="A195:A200" si="25">"29.06.2020"</f>
         <v>29.06.2020</v>
       </c>
       <c r="B195" s="12"/>
@@ -10391,7 +10396,7 @@
     </row>
     <row r="196" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A196" s="9" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>29.06.2020</v>
       </c>
       <c r="B196" s="12"/>
@@ -10417,7 +10422,7 @@
     </row>
     <row r="197" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A197" s="9" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>29.06.2020</v>
       </c>
       <c r="B197" s="12"/>
@@ -10443,7 +10448,7 @@
     </row>
     <row r="198" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A198" s="9" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>29.06.2020</v>
       </c>
       <c r="B198" s="12"/>
@@ -10469,7 +10474,7 @@
     </row>
     <row r="199" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A199" s="9" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>29.06.2020</v>
       </c>
       <c r="B199" s="12"/>
@@ -10495,7 +10500,7 @@
     </row>
     <row r="200" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A200" s="9" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>29.06.2020</v>
       </c>
       <c r="B200" s="12"/>
@@ -10547,7 +10552,7 @@
     </row>
     <row r="202" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A202" s="9" t="str">
-        <f t="shared" ref="A202:A204" si="25">"03.06.2020"</f>
+        <f t="shared" ref="A202:A204" si="26">"03.06.2020"</f>
         <v>03.06.2020</v>
       </c>
       <c r="B202" s="12"/>
@@ -10573,7 +10578,7 @@
     </row>
     <row r="203" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A203" s="9" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>03.06.2020</v>
       </c>
       <c r="B203" s="12"/>
@@ -10599,7 +10604,7 @@
     </row>
     <row r="204" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A204" s="9" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>03.06.2020</v>
       </c>
       <c r="B204" s="12"/>
@@ -10653,7 +10658,7 @@
     </row>
     <row r="206" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A206" s="9" t="str">
-        <f t="shared" ref="A206:A210" si="26">"06.05.2020"</f>
+        <f t="shared" ref="A206:A210" si="27">"06.05.2020"</f>
         <v>06.05.2020</v>
       </c>
       <c r="B206" s="12"/>
@@ -10679,7 +10684,7 @@
     </row>
     <row r="207" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A207" s="9" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>06.05.2020</v>
       </c>
       <c r="B207" s="12"/>
@@ -10705,7 +10710,7 @@
     </row>
     <row r="208" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A208" s="9" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>06.05.2020</v>
       </c>
       <c r="B208" s="12"/>
@@ -10731,7 +10736,7 @@
     </row>
     <row r="209" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A209" s="9" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>06.05.2020</v>
       </c>
       <c r="B209" s="12"/>
@@ -10757,7 +10762,7 @@
     </row>
     <row r="210" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A210" s="9" t="str">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>06.05.2020</v>
       </c>
       <c r="B210" s="12"/>
@@ -10809,7 +10814,7 @@
     </row>
     <row r="212" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A212" s="9" t="str">
-        <f t="shared" ref="A212:A216" si="27">"04.02.2020"</f>
+        <f t="shared" ref="A212:A216" si="28">"04.02.2020"</f>
         <v>04.02.2020</v>
       </c>
       <c r="B212" s="12"/>
@@ -10833,7 +10838,7 @@
     </row>
     <row r="213" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A213" s="9" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>04.02.2020</v>
       </c>
       <c r="B213" s="12"/>
@@ -10857,7 +10862,7 @@
     </row>
     <row r="214" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A214" s="9" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>04.02.2020</v>
       </c>
       <c r="B214" s="12"/>
@@ -10881,7 +10886,7 @@
     </row>
     <row r="215" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A215" s="9" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>04.02.2020</v>
       </c>
       <c r="B215" s="12"/>
@@ -10903,7 +10908,7 @@
     </row>
     <row r="216" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A216" s="9" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>04.02.2020</v>
       </c>
       <c r="B216" s="12"/>
@@ -10953,7 +10958,7 @@
     </row>
     <row r="218" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A218" s="9" t="str">
-        <f t="shared" ref="A218:A225" si="28">"01.11.2019"</f>
+        <f t="shared" ref="A218:A225" si="29">"01.11.2019"</f>
         <v>01.11.2019</v>
       </c>
       <c r="B218" s="12"/>
@@ -10977,7 +10982,7 @@
     </row>
     <row r="219" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A219" s="9" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>01.11.2019</v>
       </c>
       <c r="B219" s="12"/>
@@ -11001,7 +11006,7 @@
     </row>
     <row r="220" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A220" s="9" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>01.11.2019</v>
       </c>
       <c r="B220" s="12"/>
@@ -11025,7 +11030,7 @@
     </row>
     <row r="221" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A221" s="9" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>01.11.2019</v>
       </c>
       <c r="B221" s="12"/>
@@ -11049,7 +11054,7 @@
     </row>
     <row r="222" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A222" s="9" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>01.11.2019</v>
       </c>
       <c r="B222" s="12"/>
@@ -11070,7 +11075,7 @@
     </row>
     <row r="223" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A223" s="9" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>01.11.2019</v>
       </c>
       <c r="B223" s="12"/>
@@ -11094,7 +11099,7 @@
     </row>
     <row r="224" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A224" s="9" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>01.11.2019</v>
       </c>
       <c r="B224" s="12"/>
@@ -11118,7 +11123,7 @@
     </row>
     <row r="225" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A225" s="9" t="str">
-        <f t="shared" si="28"/>
+        <f t="shared" si="29"/>
         <v>01.11.2019</v>
       </c>
       <c r="B225" s="12"/>
@@ -11167,7 +11172,7 @@
     </row>
     <row r="227" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A227" s="9" t="str">
-        <f t="shared" ref="A227:A232" si="29">"21.08.2019"</f>
+        <f t="shared" ref="A227:A232" si="30">"21.08.2019"</f>
         <v>21.08.2019</v>
       </c>
       <c r="B227" s="12"/>
@@ -11190,7 +11195,7 @@
     </row>
     <row r="228" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A228" s="9" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>21.08.2019</v>
       </c>
       <c r="B228" s="12"/>
@@ -11210,7 +11215,7 @@
     </row>
     <row r="229" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A229" s="9" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>21.08.2019</v>
       </c>
       <c r="B229" s="12"/>
@@ -11231,7 +11236,7 @@
     </row>
     <row r="230" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A230" s="9" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>21.08.2019</v>
       </c>
       <c r="B230" s="12"/>
@@ -11252,7 +11257,7 @@
     </row>
     <row r="231" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A231" s="9" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>21.08.2019</v>
       </c>
       <c r="B231" s="12"/>
@@ -11273,7 +11278,7 @@
     </row>
     <row r="232" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A232" s="9" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>21.08.2019</v>
       </c>
       <c r="B232" s="12"/>
@@ -11318,7 +11323,7 @@
     </row>
     <row r="234" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A234" s="9" t="str">
-        <f t="shared" ref="A234:A240" si="30">"04.06.2019"</f>
+        <f t="shared" ref="A234:A240" si="31">"04.06.2019"</f>
         <v>04.06.2019</v>
       </c>
       <c r="B234" s="12"/>
@@ -11341,7 +11346,7 @@
     </row>
     <row r="235" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A235" s="9" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>04.06.2019</v>
       </c>
       <c r="B235" s="12"/>
@@ -11364,7 +11369,7 @@
     </row>
     <row r="236" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A236" s="9" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>04.06.2019</v>
       </c>
       <c r="B236" s="12"/>
@@ -11387,7 +11392,7 @@
     </row>
     <row r="237" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A237" s="9" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>04.06.2019</v>
       </c>
       <c r="B237" s="12"/>
@@ -11410,7 +11415,7 @@
     </row>
     <row r="238" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A238" s="9" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>04.06.2019</v>
       </c>
       <c r="B238" s="12"/>
@@ -11433,7 +11438,7 @@
     </row>
     <row r="239" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A239" s="9" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>04.06.2019</v>
       </c>
       <c r="B239" s="12"/>
@@ -11456,7 +11461,7 @@
     </row>
     <row r="240" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A240" s="9" t="str">
-        <f t="shared" si="30"/>
+        <f t="shared" si="31"/>
         <v>04.06.2019</v>
       </c>
       <c r="B240" s="12"/>
@@ -11504,7 +11509,7 @@
     </row>
     <row r="242" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A242" s="9" t="str">
-        <f t="shared" ref="A242:A252" si="31">"10.05.2019"</f>
+        <f t="shared" ref="A242:A252" si="32">"10.05.2019"</f>
         <v>10.05.2019</v>
       </c>
       <c r="B242" s="12"/>
@@ -11527,7 +11532,7 @@
     </row>
     <row r="243" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A243" s="9" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>10.05.2019</v>
       </c>
       <c r="B243" s="12"/>
@@ -11550,7 +11555,7 @@
     </row>
     <row r="244" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A244" s="9" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>10.05.2019</v>
       </c>
       <c r="B244" s="12"/>
@@ -11573,7 +11578,7 @@
     </row>
     <row r="245" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A245" s="9" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>10.05.2019</v>
       </c>
       <c r="B245" s="12"/>
@@ -11596,7 +11601,7 @@
     </row>
     <row r="246" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A246" s="9" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>10.05.2019</v>
       </c>
       <c r="B246" s="12"/>
@@ -11619,7 +11624,7 @@
     </row>
     <row r="247" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A247" s="9" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>10.05.2019</v>
       </c>
       <c r="B247" s="12"/>
@@ -11642,7 +11647,7 @@
     </row>
     <row r="248" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A248" s="9" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>10.05.2019</v>
       </c>
       <c r="B248" s="12"/>
@@ -11665,7 +11670,7 @@
     </row>
     <row r="249" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A249" s="9" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>10.05.2019</v>
       </c>
       <c r="B249" s="12"/>
@@ -11688,7 +11693,7 @@
     </row>
     <row r="250" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A250" s="9" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>10.05.2019</v>
       </c>
       <c r="B250" s="12"/>
@@ -11711,7 +11716,7 @@
     </row>
     <row r="251" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A251" s="9" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>10.05.2019</v>
       </c>
       <c r="B251" s="12"/>
@@ -11731,7 +11736,7 @@
     </row>
     <row r="252" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A252" s="9" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="32"/>
         <v>10.05.2019</v>
       </c>
       <c r="B252" s="12"/>
@@ -11776,7 +11781,7 @@
     </row>
     <row r="254" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A254" s="9" t="str">
-        <f t="shared" ref="A254:A261" si="32">"27.06.2018"</f>
+        <f t="shared" ref="A254:A261" si="33">"27.06.2018"</f>
         <v>27.06.2018</v>
       </c>
       <c r="B254" s="12"/>
@@ -11799,7 +11804,7 @@
     </row>
     <row r="255" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A255" s="9" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>27.06.2018</v>
       </c>
       <c r="B255" s="12"/>
@@ -11822,7 +11827,7 @@
     </row>
     <row r="256" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A256" s="9" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>27.06.2018</v>
       </c>
       <c r="B256" s="12"/>
@@ -11845,7 +11850,7 @@
     </row>
     <row r="257" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A257" s="9" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>27.06.2018</v>
       </c>
       <c r="B257" s="12"/>
@@ -11868,7 +11873,7 @@
     </row>
     <row r="258" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A258" s="9" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>27.06.2018</v>
       </c>
       <c r="B258" s="12"/>
@@ -11891,7 +11896,7 @@
     </row>
     <row r="259" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A259" s="9" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>27.06.2018</v>
       </c>
       <c r="B259" s="12"/>
@@ -11914,7 +11919,7 @@
     </row>
     <row r="260" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A260" s="9" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>27.06.2018</v>
       </c>
       <c r="B260" s="12"/>
@@ -11937,7 +11942,7 @@
     </row>
     <row r="261" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A261" s="9" t="str">
-        <f t="shared" si="32"/>
+        <f t="shared" si="33"/>
         <v>27.06.2018</v>
       </c>
       <c r="B261" s="12"/>
@@ -11985,7 +11990,7 @@
     </row>
     <row r="263" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A263" s="9" t="str">
-        <f t="shared" ref="A263:A264" si="33">"26.06.2018"</f>
+        <f t="shared" ref="A263:A264" si="34">"26.06.2018"</f>
         <v>26.06.2018</v>
       </c>
       <c r="B263" s="12"/>
@@ -12008,7 +12013,7 @@
     </row>
     <row r="264" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A264" s="9" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="34"/>
         <v>26.06.2018</v>
       </c>
       <c r="B264" s="12"/>
@@ -12056,7 +12061,7 @@
     </row>
     <row r="266" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A266" s="9" t="str">
-        <f t="shared" ref="A266:A269" si="34">"17.04.2018"</f>
+        <f t="shared" ref="A266:A269" si="35">"17.04.2018"</f>
         <v>17.04.2018</v>
       </c>
       <c r="B266" s="12"/>
@@ -12079,7 +12084,7 @@
     </row>
     <row r="267" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A267" s="9" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>17.04.2018</v>
       </c>
       <c r="B267" s="12"/>
@@ -12102,7 +12107,7 @@
     </row>
     <row r="268" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A268" s="9" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>17.04.2018</v>
       </c>
       <c r="B268" s="12"/>
@@ -12125,7 +12130,7 @@
     </row>
     <row r="269" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A269" s="9" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="35"/>
         <v>17.04.2018</v>
       </c>
       <c r="B269" s="12"/>
@@ -12173,7 +12178,7 @@
     </row>
     <row r="271" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A271" s="9" t="str">
-        <f t="shared" ref="A271:A272" si="35">"20.03.2018"</f>
+        <f t="shared" ref="A271:A272" si="36">"20.03.2018"</f>
         <v>20.03.2018</v>
       </c>
       <c r="B271" s="12"/>
@@ -12196,7 +12201,7 @@
     </row>
     <row r="272" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A272" s="9" t="str">
-        <f t="shared" si="35"/>
+        <f t="shared" si="36"/>
         <v>20.03.2018</v>
       </c>
       <c r="B272" s="12"/>
@@ -12319,7 +12324,7 @@
     </row>
     <row r="277" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A277" s="9" t="str">
-        <f t="shared" ref="A277:A283" si="36">"11.09.2017"</f>
+        <f t="shared" ref="A277:A283" si="37">"11.09.2017"</f>
         <v>11.09.2017</v>
       </c>
       <c r="B277" s="12"/>
@@ -12343,7 +12348,7 @@
     </row>
     <row r="278" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A278" s="9" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>11.09.2017</v>
       </c>
       <c r="B278" s="12"/>
@@ -12367,7 +12372,7 @@
     </row>
     <row r="279" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A279" s="9" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>11.09.2017</v>
       </c>
       <c r="B279" s="12"/>
@@ -12391,7 +12396,7 @@
     </row>
     <row r="280" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A280" s="9" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>11.09.2017</v>
       </c>
       <c r="B280" s="12"/>
@@ -12415,7 +12420,7 @@
     </row>
     <row r="281" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A281" s="9" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>11.09.2017</v>
       </c>
       <c r="B281" s="12"/>
@@ -12439,7 +12444,7 @@
     </row>
     <row r="282" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A282" s="9" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>11.09.2017</v>
       </c>
       <c r="B282" s="12"/>
@@ -12463,7 +12468,7 @@
     </row>
     <row r="283" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A283" s="9" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="37"/>
         <v>11.09.2017</v>
       </c>
       <c r="B283" s="12"/>
@@ -12513,7 +12518,7 @@
     </row>
     <row r="285" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A285" s="9" t="str">
-        <f t="shared" ref="A285:A286" si="37">"26.06.2017"</f>
+        <f t="shared" ref="A285:A286" si="38">"26.06.2017"</f>
         <v>26.06.2017</v>
       </c>
       <c r="B285" s="12"/>
@@ -12537,7 +12542,7 @@
     </row>
     <row r="286" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A286" s="9" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" si="38"/>
         <v>26.06.2017</v>
       </c>
       <c r="B286" s="12"/>
@@ -12561,7 +12566,7 @@
     </row>
     <row r="287" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A287" s="9" t="str">
-        <f t="shared" ref="A287:A295" si="38">"15.06.2017"</f>
+        <f t="shared" ref="A287:A295" si="39">"15.06.2017"</f>
         <v>15.06.2017</v>
       </c>
       <c r="B287" s="12" t="s">
@@ -12586,7 +12591,7 @@
     </row>
     <row r="288" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A288" s="9" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>15.06.2017</v>
       </c>
       <c r="B288" s="12"/>
@@ -12609,7 +12614,7 @@
     </row>
     <row r="289" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A289" s="9" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>15.06.2017</v>
       </c>
       <c r="B289" s="12"/>
@@ -12632,7 +12637,7 @@
     </row>
     <row r="290" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A290" s="9" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>15.06.2017</v>
       </c>
       <c r="B290" s="12"/>
@@ -12655,7 +12660,7 @@
     </row>
     <row r="291" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A291" s="9" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>15.06.2017</v>
       </c>
       <c r="B291" s="12"/>
@@ -12678,7 +12683,7 @@
     </row>
     <row r="292" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A292" s="9" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>15.06.2017</v>
       </c>
       <c r="B292" s="12"/>
@@ -12701,7 +12706,7 @@
     </row>
     <row r="293" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A293" s="9" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>15.06.2017</v>
       </c>
       <c r="B293" s="12"/>
@@ -12724,7 +12729,7 @@
     </row>
     <row r="294" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A294" s="9" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>15.06.2017</v>
       </c>
       <c r="B294" s="12"/>
@@ -12747,7 +12752,7 @@
     </row>
     <row r="295" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A295" s="9" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="39"/>
         <v>15.06.2017</v>
       </c>
       <c r="B295" s="12"/>
@@ -12795,7 +12800,7 @@
     </row>
     <row r="297" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A297" s="9" t="str">
-        <f t="shared" ref="A297:A301" si="39">"05.05.2017"</f>
+        <f t="shared" ref="A297:A301" si="40">"05.05.2017"</f>
         <v>05.05.2017</v>
       </c>
       <c r="B297" s="12"/>
@@ -12818,7 +12823,7 @@
     </row>
     <row r="298" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A298" s="9" t="str">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>05.05.2017</v>
       </c>
       <c r="B298" s="12"/>
@@ -12841,7 +12846,7 @@
     </row>
     <row r="299" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A299" s="9" t="str">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>05.05.2017</v>
       </c>
       <c r="B299" s="12"/>
@@ -12864,7 +12869,7 @@
     </row>
     <row r="300" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A300" s="9" t="str">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>05.05.2017</v>
       </c>
       <c r="B300" s="12"/>
@@ -12887,7 +12892,7 @@
     </row>
     <row r="301" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A301" s="9" t="str">
-        <f t="shared" si="39"/>
+        <f t="shared" si="40"/>
         <v>05.05.2017</v>
       </c>
       <c r="B301" s="12"/>
@@ -12987,7 +12992,7 @@
     </row>
     <row r="305" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A305" s="9" t="str">
-        <f t="shared" ref="A305:A308" si="40">"29.11.2016"</f>
+        <f t="shared" ref="A305:A308" si="41">"29.11.2016"</f>
         <v>29.11.2016</v>
       </c>
       <c r="B305" s="12"/>
@@ -13010,7 +13015,7 @@
     </row>
     <row r="306" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A306" s="9" t="str">
-        <f t="shared" si="40"/>
+        <f t="shared" si="41"/>
         <v>29.11.2016</v>
       </c>
       <c r="B306" s="12"/>
@@ -13033,7 +13038,7 @@
     </row>
     <row r="307" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A307" s="9" t="str">
-        <f t="shared" si="40"/>
+        <f t="shared" si="41"/>
         <v>29.11.2016</v>
       </c>
       <c r="B307" s="12"/>
@@ -13056,7 +13061,7 @@
     </row>
     <row r="308" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A308" s="9" t="str">
-        <f t="shared" si="40"/>
+        <f t="shared" si="41"/>
         <v>29.11.2016</v>
       </c>
       <c r="B308" s="12"/>
@@ -13105,7 +13110,7 @@
     </row>
     <row r="310" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A310" s="9" t="str">
-        <f t="shared" ref="A310:A312" si="41">"14.11.2016"</f>
+        <f t="shared" ref="A310:A312" si="42">"14.11.2016"</f>
         <v>14.11.2016</v>
       </c>
       <c r="B310" s="12"/>
@@ -13129,7 +13134,7 @@
     </row>
     <row r="311" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A311" s="9" t="str">
-        <f t="shared" si="41"/>
+        <f t="shared" si="42"/>
         <v>14.11.2016</v>
       </c>
       <c r="B311" s="12"/>
@@ -13153,7 +13158,7 @@
     </row>
     <row r="312" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A312" s="9" t="str">
-        <f t="shared" si="41"/>
+        <f t="shared" si="42"/>
         <v>14.11.2016</v>
       </c>
       <c r="B312" s="12"/>
@@ -13203,7 +13208,7 @@
     </row>
     <row r="314" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A314" s="9" t="str">
-        <f t="shared" ref="A314:A315" si="42">"17.10.2016"</f>
+        <f t="shared" ref="A314:A315" si="43">"17.10.2016"</f>
         <v>17.10.2016</v>
       </c>
       <c r="B314" s="12"/>
@@ -13227,7 +13232,7 @@
     </row>
     <row r="315" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A315" s="9" t="str">
-        <f t="shared" si="42"/>
+        <f t="shared" si="43"/>
         <v>17.10.2016</v>
       </c>
       <c r="B315" s="12"/>
@@ -13277,7 +13282,7 @@
     </row>
     <row r="317" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A317" s="9" t="str">
-        <f t="shared" ref="A317:A321" si="43">"14.09.2016"</f>
+        <f t="shared" ref="A317:A321" si="44">"14.09.2016"</f>
         <v>14.09.2016</v>
       </c>
       <c r="B317" s="12"/>
@@ -13301,7 +13306,7 @@
     </row>
     <row r="318" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A318" s="9" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>14.09.2016</v>
       </c>
       <c r="B318" s="12"/>
@@ -13325,7 +13330,7 @@
     </row>
     <row r="319" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A319" s="9" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>14.09.2016</v>
       </c>
       <c r="B319" s="12"/>
@@ -13349,7 +13354,7 @@
     </row>
     <row r="320" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A320" s="9" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>14.09.2016</v>
       </c>
       <c r="B320" s="12"/>
@@ -13373,7 +13378,7 @@
     </row>
     <row r="321" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A321" s="9" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="44"/>
         <v>14.09.2016</v>
       </c>
       <c r="B321" s="12"/>
@@ -13514,7 +13519,7 @@
     </row>
     <row r="327" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A327" s="9" t="str">
-        <f t="shared" ref="A327:A335" si="44">"28.04.2016"</f>
+        <f t="shared" ref="A327:A335" si="45">"28.04.2016"</f>
         <v>28.04.2016</v>
       </c>
       <c r="B327" s="12"/>
@@ -13538,7 +13543,7 @@
     </row>
     <row r="328" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A328" s="9" t="str">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v>28.04.2016</v>
       </c>
       <c r="B328" s="12"/>
@@ -13559,7 +13564,7 @@
     </row>
     <row r="329" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A329" s="9" t="str">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v>28.04.2016</v>
       </c>
       <c r="B329" s="12"/>
@@ -13583,7 +13588,7 @@
     </row>
     <row r="330" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A330" s="9" t="str">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v>28.04.2016</v>
       </c>
       <c r="B330" s="12"/>
@@ -13607,7 +13612,7 @@
     </row>
     <row r="331" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A331" s="9" t="str">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v>28.04.2016</v>
       </c>
       <c r="B331" s="12"/>
@@ -13631,7 +13636,7 @@
     </row>
     <row r="332" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A332" s="9" t="str">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v>28.04.2016</v>
       </c>
       <c r="B332" s="12"/>
@@ -13655,7 +13660,7 @@
     </row>
     <row r="333" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A333" s="9" t="str">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v>28.04.2016</v>
       </c>
       <c r="B333" s="12"/>
@@ -13677,7 +13682,7 @@
     </row>
     <row r="334" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A334" s="9" t="str">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v>28.04.2016</v>
       </c>
       <c r="B334" s="12"/>
@@ -13701,7 +13706,7 @@
     </row>
     <row r="335" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A335" s="9" t="str">
-        <f t="shared" si="44"/>
+        <f t="shared" si="45"/>
         <v>28.04.2016</v>
       </c>
       <c r="B335" s="12"/>
@@ -13749,7 +13754,7 @@
     </row>
     <row r="337" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A337" s="9" t="str">
-        <f t="shared" ref="A337:A341" si="45">"13.01.2016"</f>
+        <f t="shared" ref="A337:A341" si="46">"13.01.2016"</f>
         <v>13.01.2016</v>
       </c>
       <c r="B337" s="12"/>
@@ -13773,7 +13778,7 @@
     </row>
     <row r="338" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A338" s="9" t="str">
-        <f t="shared" si="45"/>
+        <f t="shared" si="46"/>
         <v>13.01.2016</v>
       </c>
       <c r="B338" s="12"/>
@@ -13797,7 +13802,7 @@
     </row>
     <row r="339" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A339" s="9" t="str">
-        <f t="shared" si="45"/>
+        <f t="shared" si="46"/>
         <v>13.01.2016</v>
       </c>
       <c r="B339" s="12"/>
@@ -13821,7 +13826,7 @@
     </row>
     <row r="340" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A340" s="9" t="str">
-        <f t="shared" si="45"/>
+        <f t="shared" si="46"/>
         <v>13.01.2016</v>
       </c>
       <c r="B340" s="12"/>
@@ -13843,7 +13848,7 @@
     </row>
     <row r="341" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A341" s="9" t="str">
-        <f t="shared" si="45"/>
+        <f t="shared" si="46"/>
         <v>13.01.2016</v>
       </c>
       <c r="B341" s="12"/>
@@ -13941,7 +13946,7 @@
     </row>
     <row r="345" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A345" s="9" t="str">
-        <f t="shared" ref="A345:A354" si="46">"23.06.2015"</f>
+        <f t="shared" ref="A345:A354" si="47">"23.06.2015"</f>
         <v>23.06.2015</v>
       </c>
       <c r="B345" s="12"/>
@@ -13963,7 +13968,7 @@
     </row>
     <row r="346" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A346" s="9" t="str">
-        <f t="shared" si="46"/>
+        <f t="shared" si="47"/>
         <v>23.06.2015</v>
       </c>
       <c r="B346" s="12"/>
@@ -13987,7 +13992,7 @@
     </row>
     <row r="347" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A347" s="9" t="str">
-        <f t="shared" si="46"/>
+        <f t="shared" si="47"/>
         <v>23.06.2015</v>
       </c>
       <c r="B347" s="12"/>
@@ -14011,7 +14016,7 @@
     </row>
     <row r="348" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A348" s="9" t="str">
-        <f t="shared" si="46"/>
+        <f t="shared" si="47"/>
         <v>23.06.2015</v>
       </c>
       <c r="B348" s="12"/>
@@ -14035,7 +14040,7 @@
     </row>
     <row r="349" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A349" s="9" t="str">
-        <f t="shared" si="46"/>
+        <f t="shared" si="47"/>
         <v>23.06.2015</v>
       </c>
       <c r="B349" s="12"/>
@@ -14059,7 +14064,7 @@
     </row>
     <row r="350" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A350" s="9" t="str">
-        <f t="shared" si="46"/>
+        <f t="shared" si="47"/>
         <v>23.06.2015</v>
       </c>
       <c r="B350" s="12"/>
@@ -14083,7 +14088,7 @@
     </row>
     <row r="351" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A351" s="9" t="str">
-        <f t="shared" si="46"/>
+        <f t="shared" si="47"/>
         <v>23.06.2015</v>
       </c>
       <c r="B351" s="12"/>
@@ -14107,7 +14112,7 @@
     </row>
     <row r="352" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A352" s="9" t="str">
-        <f t="shared" si="46"/>
+        <f t="shared" si="47"/>
         <v>23.06.2015</v>
       </c>
       <c r="B352" s="12"/>
@@ -14131,7 +14136,7 @@
     </row>
     <row r="353" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A353" s="9" t="str">
-        <f t="shared" si="46"/>
+        <f t="shared" si="47"/>
         <v>23.06.2015</v>
       </c>
       <c r="B353" s="12"/>
@@ -14155,7 +14160,7 @@
     </row>
     <row r="354" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A354" s="9" t="str">
-        <f t="shared" si="46"/>
+        <f t="shared" si="47"/>
         <v>23.06.2015</v>
       </c>
       <c r="B354" s="12"/>
@@ -14279,7 +14284,7 @@
     </row>
     <row r="359" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A359" s="9" t="str">
-        <f t="shared" ref="A359:A365" si="47">"13.11.2014"</f>
+        <f t="shared" ref="A359:A365" si="48">"13.11.2014"</f>
         <v>13.11.2014</v>
       </c>
       <c r="B359" s="12"/>
@@ -14303,7 +14308,7 @@
     </row>
     <row r="360" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A360" s="9" t="str">
-        <f t="shared" si="47"/>
+        <f t="shared" si="48"/>
         <v>13.11.2014</v>
       </c>
       <c r="B360" s="12"/>
@@ -14327,7 +14332,7 @@
     </row>
     <row r="361" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A361" s="9" t="str">
-        <f t="shared" si="47"/>
+        <f t="shared" si="48"/>
         <v>13.11.2014</v>
       </c>
       <c r="B361" s="12"/>
@@ -14351,7 +14356,7 @@
     </row>
     <row r="362" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A362" s="9" t="str">
-        <f t="shared" si="47"/>
+        <f t="shared" si="48"/>
         <v>13.11.2014</v>
       </c>
       <c r="B362" s="12"/>
@@ -14375,7 +14380,7 @@
     </row>
     <row r="363" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A363" s="9" t="str">
-        <f t="shared" si="47"/>
+        <f t="shared" si="48"/>
         <v>13.11.2014</v>
       </c>
       <c r="B363" s="12"/>
@@ -14399,7 +14404,7 @@
     </row>
     <row r="364" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A364" s="9" t="str">
-        <f t="shared" si="47"/>
+        <f t="shared" si="48"/>
         <v>13.11.2014</v>
       </c>
       <c r="B364" s="12"/>
@@ -14423,7 +14428,7 @@
     </row>
     <row r="365" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A365" s="9" t="str">
-        <f t="shared" si="47"/>
+        <f t="shared" si="48"/>
         <v>13.11.2014</v>
       </c>
       <c r="B365" s="12"/>
@@ -14473,7 +14478,7 @@
     </row>
     <row r="367" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A367" s="9" t="str">
-        <f t="shared" ref="A367:A372" si="48">"02.10.2014"</f>
+        <f t="shared" ref="A367:A372" si="49">"02.10.2014"</f>
         <v>02.10.2014</v>
       </c>
       <c r="B367" s="12"/>
@@ -14497,7 +14502,7 @@
     </row>
     <row r="368" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A368" s="9" t="str">
-        <f t="shared" si="48"/>
+        <f t="shared" si="49"/>
         <v>02.10.2014</v>
       </c>
       <c r="B368" s="12"/>
@@ -14521,7 +14526,7 @@
     </row>
     <row r="369" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A369" s="9" t="str">
-        <f t="shared" si="48"/>
+        <f t="shared" si="49"/>
         <v>02.10.2014</v>
       </c>
       <c r="B369" s="12"/>
@@ -14545,7 +14550,7 @@
     </row>
     <row r="370" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A370" s="9" t="str">
-        <f t="shared" si="48"/>
+        <f t="shared" si="49"/>
         <v>02.10.2014</v>
       </c>
       <c r="B370" s="12"/>
@@ -14569,7 +14574,7 @@
     </row>
     <row r="371" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A371" s="9" t="str">
-        <f t="shared" si="48"/>
+        <f t="shared" si="49"/>
         <v>02.10.2014</v>
       </c>
       <c r="B371" s="12"/>
@@ -14593,7 +14598,7 @@
     </row>
     <row r="372" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A372" s="9" t="str">
-        <f t="shared" si="48"/>
+        <f t="shared" si="49"/>
         <v>02.10.2014</v>
       </c>
       <c r="B372" s="12"/>
@@ -14781,7 +14786,7 @@
     </row>
     <row r="380" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A380" s="9" t="str">
-        <f t="shared" ref="A380:A392" si="49">"04.06.2013"</f>
+        <f t="shared" ref="A380:A392" si="50">"04.06.2013"</f>
         <v>04.06.2013</v>
       </c>
       <c r="B380" s="12"/>
@@ -14805,7 +14810,7 @@
     </row>
     <row r="381" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A381" s="9" t="str">
-        <f t="shared" si="49"/>
+        <f t="shared" si="50"/>
         <v>04.06.2013</v>
       </c>
       <c r="B381" s="12"/>
@@ -14829,7 +14834,7 @@
     </row>
     <row r="382" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A382" s="9" t="str">
-        <f t="shared" si="49"/>
+        <f t="shared" si="50"/>
         <v>04.06.2013</v>
       </c>
       <c r="B382" s="12"/>
@@ -14853,7 +14858,7 @@
     </row>
     <row r="383" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A383" s="9" t="str">
-        <f t="shared" si="49"/>
+        <f t="shared" si="50"/>
         <v>04.06.2013</v>
       </c>
       <c r="B383" s="12"/>
@@ -14877,7 +14882,7 @@
     </row>
     <row r="384" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A384" s="9" t="str">
-        <f t="shared" si="49"/>
+        <f t="shared" si="50"/>
         <v>04.06.2013</v>
       </c>
       <c r="B384" s="12"/>
@@ -14901,7 +14906,7 @@
     </row>
     <row r="385" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A385" s="9" t="str">
-        <f t="shared" si="49"/>
+        <f t="shared" si="50"/>
         <v>04.06.2013</v>
       </c>
       <c r="B385" s="12"/>
@@ -14925,7 +14930,7 @@
     </row>
     <row r="386" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A386" s="9" t="str">
-        <f t="shared" si="49"/>
+        <f t="shared" si="50"/>
         <v>04.06.2013</v>
       </c>
       <c r="B386" s="12"/>
@@ -14949,7 +14954,7 @@
     </row>
     <row r="387" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A387" s="9" t="str">
-        <f t="shared" si="49"/>
+        <f t="shared" si="50"/>
         <v>04.06.2013</v>
       </c>
       <c r="B387" s="12"/>
@@ -14973,7 +14978,7 @@
     </row>
     <row r="388" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A388" s="9" t="str">
-        <f t="shared" si="49"/>
+        <f t="shared" si="50"/>
         <v>04.06.2013</v>
       </c>
       <c r="B388" s="12"/>
@@ -14997,7 +15002,7 @@
     </row>
     <row r="389" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A389" s="9" t="str">
-        <f t="shared" si="49"/>
+        <f t="shared" si="50"/>
         <v>04.06.2013</v>
       </c>
       <c r="B389" s="12"/>
@@ -15021,7 +15026,7 @@
     </row>
     <row r="390" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A390" s="9" t="str">
-        <f t="shared" si="49"/>
+        <f t="shared" si="50"/>
         <v>04.06.2013</v>
       </c>
       <c r="B390" s="12"/>
@@ -15045,7 +15050,7 @@
     </row>
     <row r="391" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A391" s="9" t="str">
-        <f t="shared" si="49"/>
+        <f t="shared" si="50"/>
         <v>04.06.2013</v>
       </c>
       <c r="B391" s="12"/>
@@ -15069,7 +15074,7 @@
     </row>
     <row r="392" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A392" s="9" t="str">
-        <f t="shared" si="49"/>
+        <f t="shared" si="50"/>
         <v>04.06.2013</v>
       </c>
       <c r="B392" s="12"/>
@@ -15119,7 +15124,7 @@
     </row>
     <row r="394" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A394" s="9" t="str">
-        <f t="shared" ref="A394:A395" si="50">"28.11.2012"</f>
+        <f t="shared" ref="A394:A395" si="51">"28.11.2012"</f>
         <v>28.11.2012</v>
       </c>
       <c r="B394" s="12"/>
@@ -15143,7 +15148,7 @@
     </row>
     <row r="395" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A395" s="9" t="str">
-        <f t="shared" si="50"/>
+        <f t="shared" si="51"/>
         <v>28.11.2012</v>
       </c>
       <c r="B395" s="12"/>
@@ -15193,7 +15198,7 @@
     </row>
     <row r="397" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A397" s="9" t="str">
-        <f t="shared" ref="A397:A400" si="51">"25.09.2012"</f>
+        <f t="shared" ref="A397:A400" si="52">"25.09.2012"</f>
         <v>25.09.2012</v>
       </c>
       <c r="B397" s="12"/>
@@ -15217,7 +15222,7 @@
     </row>
     <row r="398" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A398" s="9" t="str">
-        <f t="shared" si="51"/>
+        <f t="shared" si="52"/>
         <v>25.09.2012</v>
       </c>
       <c r="B398" s="12"/>
@@ -15241,7 +15246,7 @@
     </row>
     <row r="399" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A399" s="9" t="str">
-        <f t="shared" si="51"/>
+        <f t="shared" si="52"/>
         <v>25.09.2012</v>
       </c>
       <c r="B399" s="12"/>
@@ -15265,7 +15270,7 @@
     </row>
     <row r="400" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A400" s="9" t="str">
-        <f t="shared" si="51"/>
+        <f t="shared" si="52"/>
         <v>25.09.2012</v>
       </c>
       <c r="B400" s="12"/>
@@ -15315,7 +15320,7 @@
     </row>
     <row r="402" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A402" s="9" t="str">
-        <f t="shared" ref="A402:A404" si="52">"09.07.2012"</f>
+        <f t="shared" ref="A402:A404" si="53">"09.07.2012"</f>
         <v>09.07.2012</v>
       </c>
       <c r="B402" s="12"/>
@@ -15339,7 +15344,7 @@
     </row>
     <row r="403" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A403" s="9" t="str">
-        <f t="shared" si="52"/>
+        <f t="shared" si="53"/>
         <v>09.07.2012</v>
       </c>
       <c r="B403" s="12"/>
@@ -15361,7 +15366,7 @@
     </row>
     <row r="404" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A404" s="9" t="str">
-        <f t="shared" si="52"/>
+        <f t="shared" si="53"/>
         <v>09.07.2012</v>
       </c>
       <c r="B404" s="12"/>
@@ -15481,7 +15486,7 @@
     </row>
     <row r="409" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A409" s="9" t="str">
-        <f t="shared" ref="A409:A415" si="53">"16.09.2011"</f>
+        <f t="shared" ref="A409:A415" si="54">"16.09.2011"</f>
         <v>16.09.2011</v>
       </c>
       <c r="B409" s="12"/>
@@ -15505,7 +15510,7 @@
     </row>
     <row r="410" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A410" s="9" t="str">
-        <f t="shared" si="53"/>
+        <f t="shared" si="54"/>
         <v>16.09.2011</v>
       </c>
       <c r="B410" s="12"/>
@@ -15529,7 +15534,7 @@
     </row>
     <row r="411" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A411" s="9" t="str">
-        <f t="shared" si="53"/>
+        <f t="shared" si="54"/>
         <v>16.09.2011</v>
       </c>
       <c r="B411" s="12"/>
@@ -15551,7 +15556,7 @@
     </row>
     <row r="412" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A412" s="9" t="str">
-        <f t="shared" si="53"/>
+        <f t="shared" si="54"/>
         <v>16.09.2011</v>
       </c>
       <c r="B412" s="12"/>
@@ -15575,7 +15580,7 @@
     </row>
     <row r="413" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A413" s="9" t="str">
-        <f t="shared" si="53"/>
+        <f t="shared" si="54"/>
         <v>16.09.2011</v>
       </c>
       <c r="B413" s="12"/>
@@ -15599,7 +15604,7 @@
     </row>
     <row r="414" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A414" s="9" t="str">
-        <f t="shared" si="53"/>
+        <f t="shared" si="54"/>
         <v>16.09.2011</v>
       </c>
       <c r="B414" s="12"/>
@@ -15621,7 +15626,7 @@
     </row>
     <row r="415" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A415" s="9" t="str">
-        <f t="shared" si="53"/>
+        <f t="shared" si="54"/>
         <v>16.09.2011</v>
       </c>
       <c r="B415" s="12"/>
@@ -15671,7 +15676,7 @@
     </row>
     <row r="417" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A417" s="9" t="str">
-        <f t="shared" ref="A417:A419" si="54">"21.07.2011"</f>
+        <f t="shared" ref="A417:A419" si="55">"21.07.2011"</f>
         <v>21.07.2011</v>
       </c>
       <c r="B417" s="12"/>
@@ -15695,7 +15700,7 @@
     </row>
     <row r="418" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A418" s="9" t="str">
-        <f t="shared" si="54"/>
+        <f t="shared" si="55"/>
         <v>21.07.2011</v>
       </c>
       <c r="B418" s="12"/>
@@ -15719,7 +15724,7 @@
     </row>
     <row r="419" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A419" s="9" t="str">
-        <f t="shared" si="54"/>
+        <f t="shared" si="55"/>
         <v>21.07.2011</v>
       </c>
       <c r="B419" s="12"/>
@@ -15769,7 +15774,7 @@
     </row>
     <row r="421" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A421" s="9" t="str">
-        <f t="shared" ref="A421:A428" si="55">"10.05.2011"</f>
+        <f t="shared" ref="A421:A428" si="56">"10.05.2011"</f>
         <v>10.05.2011</v>
       </c>
       <c r="B421" s="12"/>
@@ -15793,7 +15798,7 @@
     </row>
     <row r="422" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A422" s="9" t="str">
-        <f t="shared" si="55"/>
+        <f t="shared" si="56"/>
         <v>10.05.2011</v>
       </c>
       <c r="B422" s="12"/>
@@ -15817,7 +15822,7 @@
     </row>
     <row r="423" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A423" s="9" t="str">
-        <f t="shared" si="55"/>
+        <f t="shared" si="56"/>
         <v>10.05.2011</v>
       </c>
       <c r="B423" s="12"/>
@@ -15841,7 +15846,7 @@
     </row>
     <row r="424" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A424" s="9" t="str">
-        <f t="shared" si="55"/>
+        <f t="shared" si="56"/>
         <v>10.05.2011</v>
       </c>
       <c r="B424" s="12"/>
@@ -15865,7 +15870,7 @@
     </row>
     <row r="425" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A425" s="9" t="str">
-        <f t="shared" si="55"/>
+        <f t="shared" si="56"/>
         <v>10.05.2011</v>
       </c>
       <c r="B425" s="12"/>
@@ -15889,7 +15894,7 @@
     </row>
     <row r="426" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A426" s="9" t="str">
-        <f t="shared" si="55"/>
+        <f t="shared" si="56"/>
         <v>10.05.2011</v>
       </c>
       <c r="B426" s="12"/>
@@ -15913,7 +15918,7 @@
     </row>
     <row r="427" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A427" s="9" t="str">
-        <f t="shared" si="55"/>
+        <f t="shared" si="56"/>
         <v>10.05.2011</v>
       </c>
       <c r="B427" s="12"/>
@@ -15937,7 +15942,7 @@
     </row>
     <row r="428" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A428" s="9" t="str">
-        <f t="shared" si="55"/>
+        <f t="shared" si="56"/>
         <v>10.05.2011</v>
       </c>
       <c r="B428" s="12"/>
@@ -15987,7 +15992,7 @@
     </row>
     <row r="430" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A430" s="9" t="str">
-        <f t="shared" ref="A430:A433" si="56">"07.05.2011"</f>
+        <f t="shared" ref="A430:A433" si="57">"07.05.2011"</f>
         <v>07.05.2011</v>
       </c>
       <c r="B430" s="12"/>
@@ -16011,7 +16016,7 @@
     </row>
     <row r="431" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A431" s="9" t="str">
-        <f t="shared" si="56"/>
+        <f t="shared" si="57"/>
         <v>07.05.2011</v>
       </c>
       <c r="B431" s="12"/>
@@ -16033,7 +16038,7 @@
     </row>
     <row r="432" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A432" s="9" t="str">
-        <f t="shared" si="56"/>
+        <f t="shared" si="57"/>
         <v>07.05.2011</v>
       </c>
       <c r="B432" s="12"/>
@@ -16057,7 +16062,7 @@
     </row>
     <row r="433" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A433" s="9" t="str">
-        <f t="shared" si="56"/>
+        <f t="shared" si="57"/>
         <v>07.05.2011</v>
       </c>
       <c r="B433" s="12"/>
@@ -16202,7 +16207,7 @@
     </row>
     <row r="439" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A439" s="9" t="str">
-        <f t="shared" ref="A439:A448" si="57">"04.10.2010"</f>
+        <f t="shared" ref="A439:A448" si="58">"04.10.2010"</f>
         <v>04.10.2010</v>
       </c>
       <c r="B439" s="12"/>
@@ -16225,7 +16230,7 @@
     </row>
     <row r="440" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A440" s="9" t="str">
-        <f t="shared" si="57"/>
+        <f t="shared" si="58"/>
         <v>04.10.2010</v>
       </c>
       <c r="B440" s="12"/>
@@ -16248,7 +16253,7 @@
     </row>
     <row r="441" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A441" s="9" t="str">
-        <f t="shared" si="57"/>
+        <f t="shared" si="58"/>
         <v>04.10.2010</v>
       </c>
       <c r="B441" s="12"/>
@@ -16271,7 +16276,7 @@
     </row>
     <row r="442" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A442" s="9" t="str">
-        <f t="shared" si="57"/>
+        <f t="shared" si="58"/>
         <v>04.10.2010</v>
       </c>
       <c r="B442" s="12"/>
@@ -16295,7 +16300,7 @@
     </row>
     <row r="443" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A443" s="9" t="str">
-        <f t="shared" si="57"/>
+        <f t="shared" si="58"/>
         <v>04.10.2010</v>
       </c>
       <c r="B443" s="12"/>
@@ -16321,7 +16326,7 @@
     </row>
     <row r="444" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A444" s="9" t="str">
-        <f t="shared" si="57"/>
+        <f t="shared" si="58"/>
         <v>04.10.2010</v>
       </c>
       <c r="B444" s="12"/>
@@ -16347,7 +16352,7 @@
     </row>
     <row r="445" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A445" s="9" t="str">
-        <f t="shared" si="57"/>
+        <f t="shared" si="58"/>
         <v>04.10.2010</v>
       </c>
       <c r="B445" s="12"/>
@@ -16368,7 +16373,7 @@
     </row>
     <row r="446" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A446" s="9" t="str">
-        <f t="shared" si="57"/>
+        <f t="shared" si="58"/>
         <v>04.10.2010</v>
       </c>
       <c r="B446" s="12"/>
@@ -16394,7 +16399,7 @@
     </row>
     <row r="447" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A447" s="9" t="str">
-        <f t="shared" si="57"/>
+        <f t="shared" si="58"/>
         <v>04.10.2010</v>
       </c>
       <c r="B447" s="12"/>
@@ -16418,7 +16423,7 @@
     </row>
     <row r="448" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A448" s="9" t="str">
-        <f t="shared" si="57"/>
+        <f t="shared" si="58"/>
         <v>04.10.2010</v>
       </c>
       <c r="B448" s="12"/>
@@ -16470,7 +16475,7 @@
     </row>
     <row r="450" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A450" s="9" t="str">
-        <f t="shared" ref="A450:A455" si="58">"24.06.2010"</f>
+        <f t="shared" ref="A450:A455" si="59">"24.06.2010"</f>
         <v>24.06.2010</v>
       </c>
       <c r="B450" s="12"/>
@@ -16494,7 +16499,7 @@
     </row>
     <row r="451" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A451" s="9" t="str">
-        <f t="shared" si="58"/>
+        <f t="shared" si="59"/>
         <v>24.06.2010</v>
       </c>
       <c r="B451" s="12"/>
@@ -16518,7 +16523,7 @@
     </row>
     <row r="452" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A452" s="9" t="str">
-        <f t="shared" si="58"/>
+        <f t="shared" si="59"/>
         <v>24.06.2010</v>
       </c>
       <c r="B452" s="12"/>
@@ -16542,7 +16547,7 @@
     </row>
     <row r="453" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A453" s="9" t="str">
-        <f t="shared" si="58"/>
+        <f t="shared" si="59"/>
         <v>24.06.2010</v>
       </c>
       <c r="B453" s="12"/>
@@ -16566,7 +16571,7 @@
     </row>
     <row r="454" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A454" s="9" t="str">
-        <f t="shared" si="58"/>
+        <f t="shared" si="59"/>
         <v>24.06.2010</v>
       </c>
       <c r="B454" s="12"/>
@@ -16590,7 +16595,7 @@
     </row>
     <row r="455" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A455" s="9" t="str">
-        <f t="shared" si="58"/>
+        <f t="shared" si="59"/>
         <v>24.06.2010</v>
       </c>
       <c r="B455" s="12"/>
@@ -16692,7 +16697,7 @@
     </row>
     <row r="459" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A459" s="9" t="str">
-        <f t="shared" ref="A459:A464" si="59">"12.03.2010"</f>
+        <f t="shared" ref="A459:A464" si="60">"12.03.2010"</f>
         <v>12.03.2010</v>
       </c>
       <c r="B459" s="12"/>
@@ -16716,7 +16721,7 @@
     </row>
     <row r="460" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A460" s="9" t="str">
-        <f t="shared" si="59"/>
+        <f t="shared" si="60"/>
         <v>12.03.2010</v>
       </c>
       <c r="B460" s="12"/>
@@ -16740,7 +16745,7 @@
     </row>
     <row r="461" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A461" s="9" t="str">
-        <f t="shared" si="59"/>
+        <f t="shared" si="60"/>
         <v>12.03.2010</v>
       </c>
       <c r="B461" s="12"/>
@@ -16764,7 +16769,7 @@
     </row>
     <row r="462" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A462" s="9" t="str">
-        <f t="shared" si="59"/>
+        <f t="shared" si="60"/>
         <v>12.03.2010</v>
       </c>
       <c r="B462" s="12"/>
@@ -16788,7 +16793,7 @@
     </row>
     <row r="463" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A463" s="9" t="str">
-        <f t="shared" si="59"/>
+        <f t="shared" si="60"/>
         <v>12.03.2010</v>
       </c>
       <c r="B463" s="12"/>
@@ -16812,7 +16817,7 @@
     </row>
     <row r="464" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A464" s="9" t="str">
-        <f t="shared" si="59"/>
+        <f t="shared" si="60"/>
         <v>12.03.2010</v>
       </c>
       <c r="B464" s="12"/>

</xml_diff>